<commit_message>
update for camera ready emnlp
</commit_message>
<xml_diff>
--- a/Experimental Results.xlsx
+++ b/Experimental Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AsusIran\Desktop\Common Ground Docs\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73ABA02A-A475-428D-9343-D5195BF45D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7E6075-CA49-4741-9B7B-F0AC1A899CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="93">
   <si>
     <t># Class</t>
   </si>
@@ -452,38 +452,6 @@
     <t>F1 CG(A, B)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Flan T5 Results on Common Ground Classification from </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="20"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Event</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Flan T5 Results on Common Ground Classification from </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="20"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Gold Belief</t>
-    </r>
-  </si>
-  <si>
     <t>Flan T5 Results on Bel Classification for Bel(A) and Bel(B) with Augmentation on CT-, PS, NB (using Flan T5 for translation)</t>
   </si>
   <si>
@@ -667,6 +635,119 @@
       </rPr>
       <t>2</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Flan T5 Results on Common Ground Classification from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Gold Belief</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Event</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Context</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Flan T5 Results on Common Ground Classification from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Event </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Context</t>
+    </r>
+  </si>
+  <si>
+    <t>CG from Gold Belief + Gold Event</t>
+  </si>
+  <si>
+    <t>Some other experiments on CG Classification</t>
+  </si>
+  <si>
+    <t>CG from solely Gold Belief</t>
+  </si>
+  <si>
+    <t>CG from Gold Event No Belief, Context</t>
+  </si>
+  <si>
+    <t>CG from Gold Event No Bel, Context</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1175,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="206">
+  <cellXfs count="211">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1448,6 +1529,69 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="16" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="16" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="16" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1460,35 +1604,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="10" fontId="2" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="2" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1523,12 +1658,6 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="16" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="16" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="2" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1622,12 +1751,6 @@
     <xf numFmtId="10" fontId="2" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="16" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1637,12 +1760,6 @@
     <xf numFmtId="10" fontId="2" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="17" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1651,50 +1768,29 @@
     </xf>
     <xf numFmtId="10" fontId="17" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="2" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="17" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="17" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="17" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="17" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="17" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1987,7 +2083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DA90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:I2"/>
     </sheetView>
   </sheetViews>
@@ -2009,11 +2105,14 @@
     <col min="15" max="15" width="10" customWidth="1"/>
     <col min="17" max="17" width="11.26953125" customWidth="1"/>
     <col min="19" max="19" width="8.90625" customWidth="1"/>
-    <col min="22" max="22" width="8.453125" customWidth="1"/>
+    <col min="22" max="22" width="8.90625" customWidth="1"/>
     <col min="23" max="23" width="13.453125" customWidth="1"/>
     <col min="24" max="24" width="10.90625" customWidth="1"/>
     <col min="25" max="25" width="10.36328125" customWidth="1"/>
-    <col min="28" max="28" width="9.54296875" customWidth="1"/>
+    <col min="28" max="28" width="10.1796875" customWidth="1"/>
+    <col min="33" max="33" width="8.7265625" customWidth="1"/>
+    <col min="35" max="35" width="10.1796875" customWidth="1"/>
+    <col min="37" max="37" width="9.453125" customWidth="1"/>
     <col min="41" max="41" width="10.81640625" customWidth="1"/>
     <col min="47" max="47" width="12.81640625" customWidth="1"/>
     <col min="54" max="54" width="10.36328125" customWidth="1"/>
@@ -2053,76 +2152,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" ht="26" x14ac:dyDescent="0.6">
-      <c r="A1" s="164" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="164"/>
-      <c r="C1" s="164"/>
-      <c r="D1" s="164"/>
-      <c r="E1" s="164"/>
-      <c r="F1" s="164"/>
-      <c r="G1" s="164"/>
-      <c r="H1" s="164"/>
-      <c r="I1" s="164"/>
-      <c r="J1" s="164"/>
-      <c r="K1" s="164"/>
-      <c r="L1" s="164"/>
-      <c r="M1" s="164"/>
-      <c r="N1" s="164"/>
-      <c r="O1" s="164"/>
-      <c r="P1" s="164"/>
-      <c r="Q1" s="164"/>
-      <c r="R1" s="164"/>
-      <c r="S1" s="164"/>
-      <c r="T1" s="164"/>
-      <c r="U1" s="164"/>
-      <c r="V1" s="164"/>
+      <c r="A1" s="180" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="180"/>
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
+      <c r="F1" s="180"/>
+      <c r="G1" s="180"/>
+      <c r="H1" s="180"/>
+      <c r="I1" s="180"/>
+      <c r="J1" s="180"/>
+      <c r="K1" s="180"/>
+      <c r="L1" s="180"/>
+      <c r="M1" s="180"/>
+      <c r="N1" s="180"/>
+      <c r="O1" s="180"/>
+      <c r="P1" s="180"/>
+      <c r="Q1" s="180"/>
+      <c r="R1" s="180"/>
+      <c r="S1" s="180"/>
+      <c r="T1" s="180"/>
+      <c r="U1" s="180"/>
+      <c r="V1" s="180"/>
     </row>
     <row r="2" spans="1:66" ht="36" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A2" s="170" t="s">
+      <c r="A2" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="Z2" s="170" t="s">
+      <c r="B2" s="186"/>
+      <c r="C2" s="186"/>
+      <c r="D2" s="186"/>
+      <c r="E2" s="186"/>
+      <c r="F2" s="186"/>
+      <c r="G2" s="186"/>
+      <c r="H2" s="186"/>
+      <c r="I2" s="186"/>
+      <c r="Z2" s="186" t="s">
         <v>46</v>
       </c>
-      <c r="AA2" s="170"/>
-      <c r="AB2" s="170"/>
-      <c r="AC2" s="170"/>
-      <c r="AD2" s="170"/>
-      <c r="AE2" s="170"/>
-      <c r="AF2" s="170"/>
-      <c r="AG2" s="170"/>
-      <c r="AH2" s="170"/>
-      <c r="AI2" s="170"/>
-      <c r="AJ2" s="170"/>
-      <c r="AK2" s="170"/>
-      <c r="AL2" s="170"/>
-      <c r="AM2" s="170"/>
-      <c r="AN2" s="170"/>
-      <c r="AO2" s="170"/>
-      <c r="AP2" s="170"/>
-      <c r="AQ2" s="170"/>
-      <c r="AR2" s="170"/>
-      <c r="AS2" s="170"/>
-      <c r="AT2" s="170"/>
-      <c r="BC2" s="139" t="s">
-        <v>76</v>
-      </c>
-      <c r="BD2" s="139"/>
-      <c r="BE2" s="139"/>
-      <c r="BF2" s="139"/>
-      <c r="BG2" s="139"/>
-      <c r="BH2" s="139"/>
-      <c r="BI2" s="139"/>
-      <c r="BJ2" s="139"/>
+      <c r="AA2" s="186"/>
+      <c r="AB2" s="186"/>
+      <c r="AC2" s="186"/>
+      <c r="AD2" s="186"/>
+      <c r="AE2" s="186"/>
+      <c r="AF2" s="186"/>
+      <c r="AG2" s="186"/>
+      <c r="AH2" s="186"/>
+      <c r="AI2" s="186"/>
+      <c r="AJ2" s="186"/>
+      <c r="AK2" s="186"/>
+      <c r="AL2" s="186"/>
+      <c r="AM2" s="186"/>
+      <c r="AN2" s="186"/>
+      <c r="AO2" s="186"/>
+      <c r="AP2" s="186"/>
+      <c r="AQ2" s="186"/>
+      <c r="AR2" s="186"/>
+      <c r="AS2" s="186"/>
+      <c r="AT2" s="186"/>
+      <c r="BC2" s="157" t="s">
+        <v>74</v>
+      </c>
+      <c r="BD2" s="157"/>
+      <c r="BE2" s="157"/>
+      <c r="BF2" s="157"/>
+      <c r="BG2" s="157"/>
+      <c r="BH2" s="157"/>
+      <c r="BI2" s="157"/>
+      <c r="BJ2" s="157"/>
     </row>
     <row r="3" spans="1:66" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
@@ -2135,127 +2234,127 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
-      <c r="K3" s="175"/>
-      <c r="L3" s="175"/>
-      <c r="M3" s="175"/>
-      <c r="N3" s="175"/>
+      <c r="K3" s="191"/>
+      <c r="L3" s="191"/>
+      <c r="M3" s="191"/>
+      <c r="N3" s="191"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
     </row>
     <row r="4" spans="1:66" s="4" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
-      <c r="B4" s="133" t="s">
+      <c r="B4" s="129" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="132"/>
-      <c r="D4" s="131" t="s">
+      <c r="C4" s="128"/>
+      <c r="D4" s="127" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="132"/>
-      <c r="F4" s="133" t="s">
+      <c r="E4" s="128"/>
+      <c r="F4" s="129" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="132"/>
-      <c r="H4" s="133" t="s">
+      <c r="G4" s="128"/>
+      <c r="H4" s="129" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="132"/>
-      <c r="J4" s="133" t="s">
+      <c r="I4" s="128"/>
+      <c r="J4" s="129" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="132"/>
-      <c r="L4" s="173" t="s">
+      <c r="K4" s="128"/>
+      <c r="L4" s="189" t="s">
         <v>37</v>
       </c>
-      <c r="M4" s="174"/>
-      <c r="N4" s="173" t="s">
+      <c r="M4" s="190"/>
+      <c r="N4" s="189" t="s">
         <v>39</v>
       </c>
-      <c r="O4" s="174"/>
-      <c r="P4" s="173" t="s">
+      <c r="O4" s="190"/>
+      <c r="P4" s="189" t="s">
         <v>40</v>
       </c>
-      <c r="Q4" s="174"/>
-      <c r="R4" s="173" t="s">
+      <c r="Q4" s="190"/>
+      <c r="R4" s="189" t="s">
         <v>38</v>
       </c>
-      <c r="S4" s="174"/>
-      <c r="T4" s="173" t="s">
+      <c r="S4" s="190"/>
+      <c r="T4" s="189" t="s">
         <v>41</v>
       </c>
-      <c r="U4" s="174"/>
-      <c r="V4" s="173" t="s">
+      <c r="U4" s="190"/>
+      <c r="V4" s="189" t="s">
         <v>42</v>
       </c>
-      <c r="W4" s="174"/>
-      <c r="X4" s="133" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y4" s="132"/>
-      <c r="AC4" s="140" t="s">
+      <c r="W4" s="190"/>
+      <c r="X4" s="129" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y4" s="128"/>
+      <c r="AC4" s="158" t="s">
         <v>31</v>
       </c>
-      <c r="AD4" s="141"/>
-      <c r="AE4" s="140" t="s">
+      <c r="AD4" s="159"/>
+      <c r="AE4" s="158" t="s">
         <v>6</v>
       </c>
-      <c r="AF4" s="141"/>
-      <c r="AG4" s="140" t="s">
+      <c r="AF4" s="159"/>
+      <c r="AG4" s="158" t="s">
         <v>32</v>
       </c>
-      <c r="AH4" s="141"/>
-      <c r="AI4" s="140" t="s">
+      <c r="AH4" s="159"/>
+      <c r="AI4" s="158" t="s">
         <v>33</v>
       </c>
-      <c r="AJ4" s="141"/>
-      <c r="AK4" s="140" t="s">
+      <c r="AJ4" s="159"/>
+      <c r="AK4" s="158" t="s">
         <v>9</v>
       </c>
-      <c r="AL4" s="141"/>
-      <c r="AM4" s="140" t="s">
+      <c r="AL4" s="159"/>
+      <c r="AM4" s="158" t="s">
         <v>37</v>
       </c>
-      <c r="AN4" s="141"/>
-      <c r="AO4" s="140" t="s">
+      <c r="AN4" s="159"/>
+      <c r="AO4" s="158" t="s">
         <v>39</v>
       </c>
-      <c r="AP4" s="141"/>
-      <c r="AQ4" s="140" t="s">
+      <c r="AP4" s="159"/>
+      <c r="AQ4" s="158" t="s">
         <v>40</v>
       </c>
-      <c r="AR4" s="141"/>
-      <c r="AS4" s="140" t="s">
+      <c r="AR4" s="159"/>
+      <c r="AS4" s="158" t="s">
         <v>38</v>
       </c>
-      <c r="AT4" s="141"/>
-      <c r="AU4" s="140" t="s">
+      <c r="AT4" s="159"/>
+      <c r="AU4" s="158" t="s">
         <v>41</v>
       </c>
-      <c r="AV4" s="141"/>
-      <c r="AW4" s="140" t="s">
+      <c r="AV4" s="159"/>
+      <c r="AW4" s="158" t="s">
         <v>42</v>
       </c>
-      <c r="AX4" s="141"/>
-      <c r="AY4" s="140" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ4" s="141"/>
-      <c r="BC4" s="133" t="s">
-        <v>73</v>
-      </c>
-      <c r="BD4" s="132"/>
-      <c r="BE4" s="133" t="s">
-        <v>74</v>
-      </c>
-      <c r="BF4" s="132"/>
-      <c r="BI4" s="140" t="s">
-        <v>73</v>
-      </c>
-      <c r="BJ4" s="141"/>
-      <c r="BK4" s="140" t="s">
-        <v>74</v>
-      </c>
-      <c r="BL4" s="141"/>
+      <c r="AX4" s="159"/>
+      <c r="AY4" s="158" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ4" s="159"/>
+      <c r="BC4" s="129" t="s">
+        <v>71</v>
+      </c>
+      <c r="BD4" s="128"/>
+      <c r="BE4" s="129" t="s">
+        <v>72</v>
+      </c>
+      <c r="BF4" s="128"/>
+      <c r="BI4" s="158" t="s">
+        <v>71</v>
+      </c>
+      <c r="BJ4" s="159"/>
+      <c r="BK4" s="158" t="s">
+        <v>72</v>
+      </c>
+      <c r="BL4" s="159"/>
     </row>
     <row r="5" spans="1:66" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
@@ -2336,54 +2435,54 @@
       <c r="AB5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="AC5" s="142" t="s">
+      <c r="AC5" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="AD5" s="143"/>
-      <c r="AE5" s="142" t="s">
+      <c r="AD5" s="161"/>
+      <c r="AE5" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="AF5" s="143"/>
-      <c r="AG5" s="142" t="s">
+      <c r="AF5" s="161"/>
+      <c r="AG5" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="AH5" s="143"/>
-      <c r="AI5" s="142" t="s">
+      <c r="AH5" s="161"/>
+      <c r="AI5" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="AJ5" s="143"/>
-      <c r="AK5" s="142" t="s">
+      <c r="AJ5" s="161"/>
+      <c r="AK5" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="AL5" s="143"/>
-      <c r="AM5" s="142" t="s">
+      <c r="AL5" s="161"/>
+      <c r="AM5" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="AN5" s="143"/>
-      <c r="AO5" s="142" t="s">
+      <c r="AN5" s="161"/>
+      <c r="AO5" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="AP5" s="143"/>
-      <c r="AQ5" s="142" t="s">
+      <c r="AP5" s="161"/>
+      <c r="AQ5" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="AR5" s="143"/>
-      <c r="AS5" s="142" t="s">
+      <c r="AR5" s="161"/>
+      <c r="AS5" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="AT5" s="143"/>
-      <c r="AU5" s="142" t="s">
+      <c r="AT5" s="161"/>
+      <c r="AU5" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="AV5" s="143"/>
-      <c r="AW5" s="142" t="s">
+      <c r="AV5" s="161"/>
+      <c r="AW5" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="AX5" s="143"/>
-      <c r="AY5" s="142" t="s">
+      <c r="AX5" s="161"/>
+      <c r="AY5" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="AZ5" s="143"/>
+      <c r="AZ5" s="161"/>
       <c r="BC5" s="31" t="s">
         <v>7</v>
       </c>
@@ -2396,14 +2495,14 @@
       <c r="BF5" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="BI5" s="142" t="s">
+      <c r="BI5" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="BJ5" s="143"/>
-      <c r="BK5" s="142" t="s">
+      <c r="BJ5" s="161"/>
+      <c r="BK5" s="160" t="s">
         <v>45</v>
       </c>
-      <c r="BL5" s="143"/>
+      <c r="BL5" s="161"/>
     </row>
     <row r="6" spans="1:66" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
@@ -2508,66 +2607,66 @@
       <c r="AB6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AC6" s="137">
+      <c r="AC6" s="155">
         <f>AVERAGE(B6:C6)</f>
         <v>0.87000000000000011</v>
       </c>
-      <c r="AD6" s="138"/>
-      <c r="AE6" s="137">
+      <c r="AD6" s="156"/>
+      <c r="AE6" s="155">
         <f t="shared" ref="AE6:AE12" si="0">AVERAGE(D6:E6)</f>
         <v>0.8683333333333334</v>
       </c>
-      <c r="AF6" s="138"/>
-      <c r="AG6" s="137">
+      <c r="AF6" s="156"/>
+      <c r="AG6" s="155">
         <f t="shared" ref="AG6:AG12" si="1">AVERAGE(F6:G6)</f>
         <v>0.85499999999999998</v>
       </c>
-      <c r="AH6" s="138"/>
-      <c r="AI6" s="137">
+      <c r="AH6" s="156"/>
+      <c r="AI6" s="155">
         <f t="shared" ref="AI6:AI12" si="2">AVERAGE(H6:I6)</f>
         <v>0.875</v>
       </c>
-      <c r="AJ6" s="138"/>
-      <c r="AK6" s="137">
+      <c r="AJ6" s="156"/>
+      <c r="AK6" s="155">
         <f t="shared" ref="AK6:AK12" si="3">AVERAGE(J6:K6)</f>
         <v>0.87666666666666671</v>
       </c>
-      <c r="AL6" s="138"/>
-      <c r="AM6" s="137">
+      <c r="AL6" s="156"/>
+      <c r="AM6" s="155">
         <f t="shared" ref="AM6:AM12" si="4">AVERAGE(L6:M6)</f>
         <v>0.875</v>
       </c>
-      <c r="AN6" s="138"/>
-      <c r="AO6" s="137">
+      <c r="AN6" s="156"/>
+      <c r="AO6" s="155">
         <f t="shared" ref="AO6:AO12" si="5">AVERAGE(N6:O6)</f>
         <v>0.8833333333333333</v>
       </c>
-      <c r="AP6" s="138"/>
-      <c r="AQ6" s="137">
+      <c r="AP6" s="156"/>
+      <c r="AQ6" s="155">
         <f t="shared" ref="AQ6:AQ12" si="6">AVERAGE(P6:Q6)</f>
         <v>0.88500000000000001</v>
       </c>
-      <c r="AR6" s="138"/>
-      <c r="AS6" s="137">
+      <c r="AR6" s="156"/>
+      <c r="AS6" s="155">
         <f t="shared" ref="AS6:AS12" si="7">AVERAGE(R6:S6)</f>
         <v>0.87250000000000005</v>
       </c>
-      <c r="AT6" s="138"/>
-      <c r="AU6" s="137">
+      <c r="AT6" s="156"/>
+      <c r="AU6" s="155">
         <f t="shared" ref="AU6:AU12" si="8">AVERAGE(T6:U6)</f>
         <v>0.88500000000000001</v>
       </c>
-      <c r="AV6" s="138"/>
-      <c r="AW6" s="137">
+      <c r="AV6" s="156"/>
+      <c r="AW6" s="155">
         <f t="shared" ref="AW6:AW12" si="9">AVERAGE(V6:W6)</f>
         <v>0.88666666666666671</v>
       </c>
-      <c r="AX6" s="138"/>
-      <c r="AY6" s="137">
+      <c r="AX6" s="156"/>
+      <c r="AY6" s="155">
         <f t="shared" ref="AY6:AY12" si="10">AVERAGE(X6:Y6)</f>
         <v>0.87749999999999995</v>
       </c>
-      <c r="AZ6" s="138"/>
+      <c r="AZ6" s="156"/>
       <c r="BC6" s="46">
         <f>AVERAGE(0.87, 0.87           )</f>
         <v>0.87</v>
@@ -2584,16 +2683,16 @@
         <f>AVERAGE(0.85, 0.87             )</f>
         <v>0.86</v>
       </c>
-      <c r="BI6" s="137">
+      <c r="BI6" s="155">
         <f>AVERAGE(BC6:BD6)</f>
         <v>0.87</v>
       </c>
-      <c r="BJ6" s="138"/>
-      <c r="BK6" s="137">
+      <c r="BJ6" s="156"/>
+      <c r="BK6" s="155">
         <f>AVERAGE(BE6:BF6)</f>
         <v>0.86166666666666658</v>
       </c>
-      <c r="BL6" s="138"/>
+      <c r="BL6" s="156"/>
     </row>
     <row r="7" spans="1:66" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
@@ -2698,66 +2797,66 @@
       <c r="AB7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AC7" s="137">
+      <c r="AC7" s="155">
         <f t="shared" ref="AC7:AC12" si="11">AVERAGE(B7:C7)</f>
         <v>0.35</v>
       </c>
-      <c r="AD7" s="138"/>
-      <c r="AE7" s="137">
+      <c r="AD7" s="156"/>
+      <c r="AE7" s="155">
         <f t="shared" si="0"/>
         <v>0.34666666666666668</v>
       </c>
-      <c r="AF7" s="138"/>
-      <c r="AG7" s="137">
+      <c r="AF7" s="156"/>
+      <c r="AG7" s="155">
         <f t="shared" si="1"/>
         <v>0.27</v>
       </c>
-      <c r="AH7" s="138"/>
-      <c r="AI7" s="137">
+      <c r="AH7" s="156"/>
+      <c r="AI7" s="155">
         <f t="shared" si="2"/>
         <v>0.27500000000000002</v>
       </c>
-      <c r="AJ7" s="138"/>
-      <c r="AK7" s="137">
+      <c r="AJ7" s="156"/>
+      <c r="AK7" s="155">
         <f t="shared" si="3"/>
         <v>0.32666666666666666</v>
       </c>
-      <c r="AL7" s="138"/>
-      <c r="AM7" s="137">
+      <c r="AL7" s="156"/>
+      <c r="AM7" s="155">
         <f t="shared" si="4"/>
         <v>0.26500000000000001</v>
       </c>
-      <c r="AN7" s="138"/>
-      <c r="AO7" s="137">
+      <c r="AN7" s="156"/>
+      <c r="AO7" s="155">
         <f t="shared" si="5"/>
         <v>0.33999999999999997</v>
       </c>
-      <c r="AP7" s="138"/>
-      <c r="AQ7" s="137">
+      <c r="AP7" s="156"/>
+      <c r="AQ7" s="155">
         <f t="shared" si="6"/>
         <v>0.31999999999999995</v>
       </c>
-      <c r="AR7" s="138"/>
-      <c r="AS7" s="137">
+      <c r="AR7" s="156"/>
+      <c r="AS7" s="155">
         <f t="shared" si="7"/>
         <v>0.24249999999999999</v>
       </c>
-      <c r="AT7" s="138"/>
-      <c r="AU7" s="137">
+      <c r="AT7" s="156"/>
+      <c r="AU7" s="155">
         <f t="shared" si="8"/>
         <v>0.15666666666666668</v>
       </c>
-      <c r="AV7" s="138"/>
-      <c r="AW7" s="137">
+      <c r="AV7" s="156"/>
+      <c r="AW7" s="155">
         <f t="shared" si="9"/>
         <v>0.32333333333333336</v>
       </c>
-      <c r="AX7" s="138"/>
-      <c r="AY7" s="137">
+      <c r="AX7" s="156"/>
+      <c r="AY7" s="155">
         <f t="shared" si="10"/>
         <v>0.27500000000000002</v>
       </c>
-      <c r="AZ7" s="138"/>
+      <c r="AZ7" s="156"/>
       <c r="BC7" s="46">
         <f>AVERAGE(0.2, 0.18         )</f>
         <v>0.19</v>
@@ -2774,16 +2873,16 @@
         <f>AVERAGE(0.13, 0.14          )</f>
         <v>0.13500000000000001</v>
       </c>
-      <c r="BI7" s="137">
+      <c r="BI7" s="155">
         <f t="shared" ref="BI7:BI8" si="12">AVERAGE(BC7:BD7)</f>
         <v>0.20250000000000001</v>
       </c>
-      <c r="BJ7" s="138"/>
-      <c r="BK7" s="137">
+      <c r="BJ7" s="156"/>
+      <c r="BK7" s="155">
         <f t="shared" ref="BK7:BK8" si="13">AVERAGE(BE7:BF7)</f>
         <v>0.1125</v>
       </c>
-      <c r="BL7" s="138"/>
+      <c r="BL7" s="156"/>
     </row>
     <row r="8" spans="1:66" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
@@ -2888,66 +2987,66 @@
       <c r="AB8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AC8" s="137">
+      <c r="AC8" s="155">
         <f t="shared" si="11"/>
         <v>0.28500000000000003</v>
       </c>
-      <c r="AD8" s="138"/>
-      <c r="AE8" s="137">
+      <c r="AD8" s="156"/>
+      <c r="AE8" s="155">
         <f t="shared" si="0"/>
         <v>0.28666666666666668</v>
       </c>
-      <c r="AF8" s="138"/>
-      <c r="AG8" s="137">
+      <c r="AF8" s="156"/>
+      <c r="AG8" s="155">
         <f t="shared" si="1"/>
         <v>0.26</v>
       </c>
-      <c r="AH8" s="138"/>
-      <c r="AI8" s="137">
+      <c r="AH8" s="156"/>
+      <c r="AI8" s="155">
         <f t="shared" si="2"/>
         <v>0.255</v>
       </c>
-      <c r="AJ8" s="138"/>
-      <c r="AK8" s="137">
+      <c r="AJ8" s="156"/>
+      <c r="AK8" s="155">
         <f t="shared" si="3"/>
         <v>0.30666666666666664</v>
       </c>
-      <c r="AL8" s="138"/>
-      <c r="AM8" s="137">
+      <c r="AL8" s="156"/>
+      <c r="AM8" s="155">
         <f t="shared" si="4"/>
         <v>0.26500000000000001</v>
       </c>
-      <c r="AN8" s="138"/>
-      <c r="AO8" s="137">
+      <c r="AN8" s="156"/>
+      <c r="AO8" s="155">
         <f t="shared" si="5"/>
         <v>0.32666666666666666</v>
       </c>
-      <c r="AP8" s="138"/>
-      <c r="AQ8" s="137">
+      <c r="AP8" s="156"/>
+      <c r="AQ8" s="155">
         <f t="shared" si="6"/>
         <v>0.3175</v>
       </c>
-      <c r="AR8" s="138"/>
-      <c r="AS8" s="137">
+      <c r="AR8" s="156"/>
+      <c r="AS8" s="155">
         <f t="shared" si="7"/>
         <v>0.28499999999999998</v>
       </c>
-      <c r="AT8" s="138"/>
-      <c r="AU8" s="137">
+      <c r="AT8" s="156"/>
+      <c r="AU8" s="155">
         <f t="shared" si="8"/>
         <v>0.26500000000000001</v>
       </c>
-      <c r="AV8" s="138"/>
-      <c r="AW8" s="137">
+      <c r="AV8" s="156"/>
+      <c r="AW8" s="155">
         <f t="shared" si="9"/>
         <v>0.28666666666666668</v>
       </c>
-      <c r="AX8" s="138"/>
-      <c r="AY8" s="137">
+      <c r="AX8" s="156"/>
+      <c r="AY8" s="155">
         <f t="shared" si="10"/>
         <v>0.3075</v>
       </c>
-      <c r="AZ8" s="138"/>
+      <c r="AZ8" s="156"/>
       <c r="BC8" s="46">
         <f>AVERAGE(0.24, 0.25            )</f>
         <v>0.245</v>
@@ -2964,16 +3063,16 @@
         <f>AVERAGE(0.17,0.09           )</f>
         <v>0.13</v>
       </c>
-      <c r="BI8" s="137">
+      <c r="BI8" s="155">
         <f t="shared" si="12"/>
         <v>0.20250000000000001</v>
       </c>
-      <c r="BJ8" s="138"/>
-      <c r="BK8" s="137">
+      <c r="BJ8" s="156"/>
+      <c r="BK8" s="155">
         <f t="shared" si="13"/>
         <v>0.18666666666666665</v>
       </c>
-      <c r="BL8" s="138"/>
+      <c r="BL8" s="156"/>
     </row>
     <row r="9" spans="1:66" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
@@ -3078,66 +3177,66 @@
       <c r="AB9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AC9" s="137">
+      <c r="AC9" s="155">
         <f t="shared" si="11"/>
         <v>0.13333333333333336</v>
       </c>
-      <c r="AD9" s="138"/>
-      <c r="AE9" s="137">
+      <c r="AD9" s="156"/>
+      <c r="AE9" s="155">
         <f t="shared" si="0"/>
         <v>0.17499999999999999</v>
       </c>
-      <c r="AF9" s="138"/>
-      <c r="AG9" s="137">
+      <c r="AF9" s="156"/>
+      <c r="AG9" s="155">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="AH9" s="138"/>
-      <c r="AI9" s="137">
+      <c r="AH9" s="156"/>
+      <c r="AI9" s="155">
         <f t="shared" si="2"/>
         <v>0.11</v>
       </c>
-      <c r="AJ9" s="138"/>
-      <c r="AK9" s="137">
+      <c r="AJ9" s="156"/>
+      <c r="AK9" s="155">
         <f t="shared" si="3"/>
         <v>0.17833333333333334</v>
       </c>
-      <c r="AL9" s="138"/>
-      <c r="AM9" s="137">
+      <c r="AL9" s="156"/>
+      <c r="AM9" s="155">
         <f t="shared" si="4"/>
         <v>0.16166666666666665</v>
       </c>
-      <c r="AN9" s="138"/>
-      <c r="AO9" s="137">
+      <c r="AN9" s="156"/>
+      <c r="AO9" s="155">
         <f t="shared" si="5"/>
         <v>0.19</v>
       </c>
-      <c r="AP9" s="138"/>
-      <c r="AQ9" s="137">
+      <c r="AP9" s="156"/>
+      <c r="AQ9" s="155">
         <f t="shared" si="6"/>
         <v>8.249999999999999E-2</v>
       </c>
-      <c r="AR9" s="138"/>
-      <c r="AS9" s="137">
+      <c r="AR9" s="156"/>
+      <c r="AS9" s="155">
         <f t="shared" si="7"/>
         <v>0.1925</v>
       </c>
-      <c r="AT9" s="138"/>
-      <c r="AU9" s="137">
+      <c r="AT9" s="156"/>
+      <c r="AU9" s="155">
         <f t="shared" si="8"/>
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="AV9" s="138"/>
-      <c r="AW9" s="137">
+      <c r="AV9" s="156"/>
+      <c r="AW9" s="155">
         <f t="shared" si="9"/>
         <v>0.11833333333333333</v>
       </c>
-      <c r="AX9" s="138"/>
-      <c r="AY9" s="137">
+      <c r="AX9" s="156"/>
+      <c r="AY9" s="155">
         <f t="shared" si="10"/>
         <v>0.1275</v>
       </c>
-      <c r="AZ9" s="138"/>
+      <c r="AZ9" s="156"/>
       <c r="BC9" s="46">
         <f>AVERAGE(0.2, 0          )</f>
         <v>0.1</v>
@@ -3154,16 +3253,16 @@
         <f>AVERAGE(0,0          )</f>
         <v>0</v>
       </c>
-      <c r="BI9" s="137">
+      <c r="BI9" s="155">
         <f>AVERAGE(BC9:BD9)</f>
         <v>0.10500000000000001</v>
       </c>
-      <c r="BJ9" s="138"/>
-      <c r="BK9" s="146">
+      <c r="BJ9" s="156"/>
+      <c r="BK9" s="164">
         <f>AVERAGE(BE9:BF9)</f>
         <v>5.5E-2</v>
       </c>
-      <c r="BL9" s="147"/>
+      <c r="BL9" s="165"/>
     </row>
     <row r="10" spans="1:66" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
@@ -3268,66 +3367,66 @@
       <c r="AB10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AC10" s="144">
+      <c r="AC10" s="162">
         <f t="shared" si="11"/>
         <v>0.74666666666666659</v>
       </c>
-      <c r="AD10" s="145"/>
-      <c r="AE10" s="144">
+      <c r="AD10" s="163"/>
+      <c r="AE10" s="162">
         <f t="shared" si="0"/>
         <v>0.74666666666666659</v>
       </c>
-      <c r="AF10" s="145"/>
-      <c r="AG10" s="144">
+      <c r="AF10" s="163"/>
+      <c r="AG10" s="162">
         <f t="shared" si="1"/>
         <v>0.72</v>
       </c>
-      <c r="AH10" s="145"/>
-      <c r="AI10" s="144">
+      <c r="AH10" s="163"/>
+      <c r="AI10" s="162">
         <f t="shared" si="2"/>
         <v>0.74</v>
       </c>
-      <c r="AJ10" s="145"/>
-      <c r="AK10" s="144">
+      <c r="AJ10" s="163"/>
+      <c r="AK10" s="162">
         <f t="shared" si="3"/>
         <v>0.76333333333333342</v>
       </c>
-      <c r="AL10" s="145"/>
-      <c r="AM10" s="144">
+      <c r="AL10" s="163"/>
+      <c r="AM10" s="162">
         <f t="shared" si="4"/>
         <v>0.75</v>
       </c>
-      <c r="AN10" s="145"/>
-      <c r="AO10" s="144">
+      <c r="AN10" s="163"/>
+      <c r="AO10" s="162">
         <f t="shared" si="5"/>
         <v>0.77833333333333332</v>
       </c>
-      <c r="AP10" s="145"/>
-      <c r="AQ10" s="144">
+      <c r="AP10" s="163"/>
+      <c r="AQ10" s="162">
         <f t="shared" si="6"/>
         <v>0.77</v>
       </c>
-      <c r="AR10" s="145"/>
-      <c r="AS10" s="144">
+      <c r="AR10" s="163"/>
+      <c r="AS10" s="162">
         <f t="shared" si="7"/>
         <v>0.74249999999999994</v>
       </c>
-      <c r="AT10" s="145"/>
-      <c r="AU10" s="144">
+      <c r="AT10" s="163"/>
+      <c r="AU10" s="162">
         <f t="shared" si="8"/>
         <v>0.7583333333333333</v>
       </c>
-      <c r="AV10" s="145"/>
-      <c r="AW10" s="144">
+      <c r="AV10" s="163"/>
+      <c r="AW10" s="162">
         <f t="shared" si="9"/>
         <v>0.76</v>
       </c>
-      <c r="AX10" s="145"/>
-      <c r="AY10" s="144">
+      <c r="AX10" s="163"/>
+      <c r="AY10" s="162">
         <f t="shared" si="10"/>
         <v>0.76249999999999996</v>
       </c>
-      <c r="AZ10" s="145"/>
+      <c r="AZ10" s="163"/>
       <c r="BB10" s="2" t="s">
         <v>5</v>
       </c>
@@ -3347,16 +3446,16 @@
         <f>AVERAGE(0.73, 0.75        )</f>
         <v>0.74</v>
       </c>
-      <c r="BI10" s="144">
+      <c r="BI10" s="162">
         <f>AVERAGE(BC10:BD10)</f>
         <v>0.76750000000000007</v>
       </c>
-      <c r="BJ10" s="145"/>
-      <c r="BK10" s="144">
+      <c r="BJ10" s="163"/>
+      <c r="BK10" s="162">
         <f>AVERAGE(BE10:BF10)</f>
         <v>0.73750000000000004</v>
       </c>
-      <c r="BL10" s="145"/>
+      <c r="BL10" s="163"/>
     </row>
     <row r="11" spans="1:66" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
@@ -3461,66 +3560,66 @@
       <c r="AB11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AC11" s="148">
+      <c r="AC11" s="137">
         <f>AVERAGE(AC6:AD9)</f>
         <v>0.40958333333333341</v>
       </c>
-      <c r="AD11" s="149"/>
-      <c r="AE11" s="148">
+      <c r="AD11" s="138"/>
+      <c r="AE11" s="137">
         <f>AVERAGE(AE6:AF9)</f>
         <v>0.41916666666666669</v>
       </c>
-      <c r="AF11" s="149"/>
-      <c r="AG11" s="148">
+      <c r="AF11" s="138"/>
+      <c r="AG11" s="137">
         <f>AVERAGE(AG6:AH9)</f>
         <v>0.39624999999999999</v>
       </c>
-      <c r="AH11" s="149"/>
-      <c r="AI11" s="148">
+      <c r="AH11" s="138"/>
+      <c r="AI11" s="137">
         <f>AVERAGE(AI6:AJ9)</f>
         <v>0.37874999999999998</v>
       </c>
-      <c r="AJ11" s="149"/>
-      <c r="AK11" s="148">
+      <c r="AJ11" s="138"/>
+      <c r="AK11" s="137">
         <f>AVERAGE(AK6:AL9)</f>
         <v>0.42208333333333337</v>
       </c>
-      <c r="AL11" s="149"/>
-      <c r="AM11" s="148">
+      <c r="AL11" s="138"/>
+      <c r="AM11" s="137">
         <f>AVERAGE(AM6:AN9)</f>
         <v>0.39166666666666672</v>
       </c>
-      <c r="AN11" s="149"/>
-      <c r="AO11" s="148">
+      <c r="AN11" s="138"/>
+      <c r="AO11" s="137">
         <f>AVERAGE(AO6:AP9)</f>
         <v>0.43499999999999994</v>
       </c>
-      <c r="AP11" s="149"/>
-      <c r="AQ11" s="148">
+      <c r="AP11" s="138"/>
+      <c r="AQ11" s="137">
         <f>AVERAGE(AQ6:AR9)</f>
         <v>0.40125</v>
       </c>
-      <c r="AR11" s="149"/>
-      <c r="AS11" s="148">
+      <c r="AR11" s="138"/>
+      <c r="AS11" s="137">
         <f>AVERAGE(AS6:AT9)</f>
         <v>0.39812499999999995</v>
       </c>
-      <c r="AT11" s="149"/>
-      <c r="AU11" s="148">
+      <c r="AT11" s="138"/>
+      <c r="AU11" s="137">
         <f>AVERAGE(AU6:AV9)</f>
         <v>0.34791666666666665</v>
       </c>
-      <c r="AV11" s="149"/>
-      <c r="AW11" s="148">
+      <c r="AV11" s="138"/>
+      <c r="AW11" s="137">
         <f>AVERAGE(AW6:AX9)</f>
         <v>0.40375</v>
       </c>
-      <c r="AX11" s="149"/>
-      <c r="AY11" s="148">
+      <c r="AX11" s="138"/>
+      <c r="AY11" s="137">
         <f>AVERAGE(AY6:AZ9)</f>
         <v>0.39687499999999998</v>
       </c>
-      <c r="AZ11" s="149"/>
+      <c r="AZ11" s="138"/>
       <c r="BB11" s="2" t="s">
         <v>43</v>
       </c>
@@ -3540,16 +3639,16 @@
         <f>AVERAGE(BF6:BF9)</f>
         <v>0.28125</v>
       </c>
-      <c r="BI11" s="148">
+      <c r="BI11" s="137">
         <f>AVERAGE(BC11:BD11)</f>
         <v>0.34500000000000003</v>
       </c>
-      <c r="BJ11" s="149"/>
-      <c r="BK11" s="148">
+      <c r="BJ11" s="138"/>
+      <c r="BK11" s="137">
         <f>AVERAGE(BE11:BF11)</f>
         <v>0.30395833333333333</v>
       </c>
-      <c r="BL11" s="149"/>
+      <c r="BL11" s="138"/>
     </row>
     <row r="12" spans="1:66" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
@@ -3654,66 +3753,66 @@
       <c r="AB12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AC12" s="134">
+      <c r="AC12" s="150">
         <f t="shared" si="11"/>
         <v>0.77333333333333343</v>
       </c>
-      <c r="AD12" s="135"/>
-      <c r="AE12" s="134">
+      <c r="AD12" s="151"/>
+      <c r="AE12" s="150">
         <f t="shared" si="0"/>
         <v>0.77333333333333343</v>
       </c>
-      <c r="AF12" s="135"/>
-      <c r="AG12" s="134">
+      <c r="AF12" s="151"/>
+      <c r="AG12" s="150">
         <f t="shared" si="1"/>
         <v>0.755</v>
       </c>
-      <c r="AH12" s="135"/>
-      <c r="AI12" s="134">
+      <c r="AH12" s="151"/>
+      <c r="AI12" s="150">
         <f t="shared" si="2"/>
         <v>0.76500000000000001</v>
       </c>
-      <c r="AJ12" s="135"/>
-      <c r="AK12" s="134">
+      <c r="AJ12" s="151"/>
+      <c r="AK12" s="150">
         <f t="shared" si="3"/>
         <v>0.77666666666666662</v>
       </c>
-      <c r="AL12" s="135"/>
-      <c r="AM12" s="134">
+      <c r="AL12" s="151"/>
+      <c r="AM12" s="150">
         <f t="shared" si="4"/>
         <v>0.76333333333333342</v>
       </c>
-      <c r="AN12" s="135"/>
-      <c r="AO12" s="134">
+      <c r="AN12" s="151"/>
+      <c r="AO12" s="150">
         <f t="shared" si="5"/>
         <v>0.78499999999999992</v>
       </c>
-      <c r="AP12" s="135"/>
-      <c r="AQ12" s="134">
+      <c r="AP12" s="151"/>
+      <c r="AQ12" s="150">
         <f t="shared" si="6"/>
         <v>0.78</v>
       </c>
-      <c r="AR12" s="135"/>
-      <c r="AS12" s="134">
+      <c r="AR12" s="151"/>
+      <c r="AS12" s="150">
         <f t="shared" si="7"/>
         <v>0.76249999999999996</v>
       </c>
-      <c r="AT12" s="135"/>
-      <c r="AU12" s="134">
+      <c r="AT12" s="151"/>
+      <c r="AU12" s="150">
         <f t="shared" si="8"/>
         <v>0.76000000000000012</v>
       </c>
-      <c r="AV12" s="135"/>
-      <c r="AW12" s="134">
+      <c r="AV12" s="151"/>
+      <c r="AW12" s="150">
         <f t="shared" si="9"/>
         <v>0.78166666666666673</v>
       </c>
-      <c r="AX12" s="135"/>
-      <c r="AY12" s="134">
+      <c r="AX12" s="151"/>
+      <c r="AY12" s="150">
         <f t="shared" si="10"/>
         <v>0.77249999999999996</v>
       </c>
-      <c r="AZ12" s="135"/>
+      <c r="AZ12" s="151"/>
       <c r="BB12" s="2" t="s">
         <v>44</v>
       </c>
@@ -3733,39 +3832,39 @@
         <f>AVERAGE(0.72, 0.74        )</f>
         <v>0.73</v>
       </c>
-      <c r="BI12" s="134">
+      <c r="BI12" s="150">
         <f>AVERAGE(BC12:BD12)</f>
         <v>0.75249999999999995</v>
       </c>
-      <c r="BJ12" s="135"/>
-      <c r="BK12" s="134">
+      <c r="BJ12" s="151"/>
+      <c r="BK12" s="150">
         <f>AVERAGE(BE12:BF12)</f>
         <v>0.72499999999999998</v>
       </c>
-      <c r="BL12" s="135"/>
+      <c r="BL12" s="151"/>
     </row>
     <row r="16" spans="1:66" ht="33.5" x14ac:dyDescent="0.75">
-      <c r="A16" s="170" t="s">
+      <c r="A16" s="186" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="170"/>
-      <c r="C16" s="170"/>
-      <c r="D16" s="170"/>
-      <c r="E16" s="170"/>
+      <c r="B16" s="186"/>
+      <c r="C16" s="186"/>
+      <c r="D16" s="186"/>
+      <c r="E16" s="186"/>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
-      <c r="AC16" s="170" t="s">
+      <c r="AC16" s="186" t="s">
         <v>48</v>
       </c>
-      <c r="AD16" s="170"/>
-      <c r="AE16" s="170"/>
-      <c r="AF16" s="170"/>
-      <c r="AG16" s="170"/>
-      <c r="AH16" s="170"/>
-      <c r="AI16" s="170"/>
-      <c r="AJ16" s="170"/>
+      <c r="AD16" s="186"/>
+      <c r="AE16" s="186"/>
+      <c r="AF16" s="186"/>
+      <c r="AG16" s="186"/>
+      <c r="AH16" s="186"/>
+      <c r="AI16" s="186"/>
+      <c r="AJ16" s="186"/>
       <c r="AK16" s="33"/>
       <c r="AL16" s="33"/>
       <c r="AM16" s="33"/>
@@ -3776,20 +3875,20 @@
       <c r="AR16" s="33"/>
       <c r="AS16" s="33"/>
       <c r="AT16" s="33"/>
-      <c r="BC16" s="130" t="s">
-        <v>77</v>
-      </c>
-      <c r="BD16" s="130"/>
-      <c r="BE16" s="130"/>
-      <c r="BF16" s="130"/>
-      <c r="BG16" s="130"/>
-      <c r="BH16" s="130"/>
-      <c r="BI16" s="130"/>
-      <c r="BJ16" s="130"/>
-      <c r="BK16" s="130"/>
-      <c r="BL16" s="130"/>
-      <c r="BM16" s="130"/>
-      <c r="BN16" s="130"/>
+      <c r="BC16" s="126" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD16" s="126"/>
+      <c r="BE16" s="126"/>
+      <c r="BF16" s="126"/>
+      <c r="BG16" s="126"/>
+      <c r="BH16" s="126"/>
+      <c r="BI16" s="126"/>
+      <c r="BJ16" s="126"/>
+      <c r="BK16" s="126"/>
+      <c r="BL16" s="126"/>
+      <c r="BM16" s="126"/>
+      <c r="BN16" s="126"/>
     </row>
     <row r="17" spans="1:105" ht="21" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A17" s="4"/>
@@ -3802,222 +3901,222 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="AC17" s="30"/>
-      <c r="BC17" s="201" t="s">
+      <c r="BC17" s="152" t="s">
+        <v>77</v>
+      </c>
+      <c r="BD17" s="153"/>
+      <c r="BE17" s="153"/>
+      <c r="BF17" s="153"/>
+      <c r="BG17" s="153"/>
+      <c r="BH17" s="154"/>
+      <c r="BI17" s="152" t="s">
+        <v>78</v>
+      </c>
+      <c r="BJ17" s="153"/>
+      <c r="BK17" s="153"/>
+      <c r="BL17" s="153"/>
+      <c r="BM17" s="153"/>
+      <c r="BN17" s="154"/>
+      <c r="BO17" s="152" t="s">
+        <v>76</v>
+      </c>
+      <c r="BP17" s="153"/>
+      <c r="BQ17" s="153"/>
+      <c r="BR17" s="153"/>
+      <c r="BS17" s="153"/>
+      <c r="BT17" s="154"/>
+      <c r="BU17" s="140" t="s">
         <v>79</v>
       </c>
-      <c r="BD17" s="202"/>
-      <c r="BE17" s="202"/>
-      <c r="BF17" s="202"/>
-      <c r="BG17" s="202"/>
-      <c r="BH17" s="203"/>
-      <c r="BI17" s="201" t="s">
-        <v>80</v>
-      </c>
-      <c r="BJ17" s="202"/>
-      <c r="BK17" s="202"/>
-      <c r="BL17" s="202"/>
-      <c r="BM17" s="202"/>
-      <c r="BN17" s="203"/>
-      <c r="BO17" s="201" t="s">
+      <c r="BV17" s="141"/>
+      <c r="BW17" s="141"/>
+      <c r="BX17" s="141"/>
+      <c r="BY17" s="141"/>
+      <c r="BZ17" s="142"/>
+      <c r="CD17" s="130" t="s">
+        <v>77</v>
+      </c>
+      <c r="CE17" s="131"/>
+      <c r="CF17" s="131"/>
+      <c r="CG17" s="131"/>
+      <c r="CH17" s="131"/>
+      <c r="CI17" s="132"/>
+      <c r="CJ17" s="130" t="s">
         <v>78</v>
       </c>
-      <c r="BP17" s="202"/>
-      <c r="BQ17" s="202"/>
-      <c r="BR17" s="202"/>
-      <c r="BS17" s="202"/>
-      <c r="BT17" s="203"/>
-      <c r="BU17" s="194" t="s">
-        <v>81</v>
-      </c>
-      <c r="BV17" s="195"/>
-      <c r="BW17" s="195"/>
-      <c r="BX17" s="195"/>
-      <c r="BY17" s="195"/>
-      <c r="BZ17" s="196"/>
-      <c r="CD17" s="191" t="s">
+      <c r="CK17" s="131"/>
+      <c r="CL17" s="131"/>
+      <c r="CM17" s="131"/>
+      <c r="CN17" s="131"/>
+      <c r="CO17" s="132"/>
+      <c r="CP17" s="130" t="s">
+        <v>76</v>
+      </c>
+      <c r="CQ17" s="131"/>
+      <c r="CR17" s="131"/>
+      <c r="CS17" s="131"/>
+      <c r="CT17" s="131"/>
+      <c r="CU17" s="132"/>
+      <c r="CV17" s="140" t="s">
         <v>79</v>
       </c>
-      <c r="CE17" s="192"/>
-      <c r="CF17" s="192"/>
-      <c r="CG17" s="192"/>
-      <c r="CH17" s="192"/>
-      <c r="CI17" s="193"/>
-      <c r="CJ17" s="191" t="s">
-        <v>80</v>
-      </c>
-      <c r="CK17" s="192"/>
-      <c r="CL17" s="192"/>
-      <c r="CM17" s="192"/>
-      <c r="CN17" s="192"/>
-      <c r="CO17" s="193"/>
-      <c r="CP17" s="191" t="s">
-        <v>78</v>
-      </c>
-      <c r="CQ17" s="192"/>
-      <c r="CR17" s="192"/>
-      <c r="CS17" s="192"/>
-      <c r="CT17" s="192"/>
-      <c r="CU17" s="193"/>
-      <c r="CV17" s="194" t="s">
-        <v>81</v>
-      </c>
-      <c r="CW17" s="195"/>
-      <c r="CX17" s="195"/>
-      <c r="CY17" s="195"/>
-      <c r="CZ17" s="195"/>
-      <c r="DA17" s="196"/>
+      <c r="CW17" s="141"/>
+      <c r="CX17" s="141"/>
+      <c r="CY17" s="141"/>
+      <c r="CZ17" s="141"/>
+      <c r="DA17" s="142"/>
     </row>
     <row r="18" spans="1:105" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
-      <c r="B18" s="133" t="s">
+      <c r="B18" s="129" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="132"/>
-      <c r="D18" s="133" t="s">
+      <c r="C18" s="128"/>
+      <c r="D18" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="132"/>
-      <c r="F18" s="133" t="s">
+      <c r="E18" s="128"/>
+      <c r="F18" s="129" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="132"/>
-      <c r="H18" s="133" t="s">
+      <c r="G18" s="128"/>
+      <c r="H18" s="129" t="s">
         <v>9</v>
       </c>
-      <c r="I18" s="132"/>
+      <c r="I18" s="128"/>
       <c r="K18" s="10"/>
-      <c r="L18" s="171" t="s">
+      <c r="L18" s="187" t="s">
         <v>10</v>
       </c>
-      <c r="M18" s="171"/>
-      <c r="N18" s="171" t="s">
+      <c r="M18" s="187"/>
+      <c r="N18" s="187" t="s">
         <v>11</v>
       </c>
-      <c r="O18" s="171"/>
+      <c r="O18" s="187"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="10"/>
-      <c r="S18" s="171" t="s">
+      <c r="S18" s="187" t="s">
         <v>15</v>
       </c>
-      <c r="T18" s="171"/>
-      <c r="U18" s="171" t="s">
+      <c r="T18" s="187"/>
+      <c r="U18" s="187" t="s">
         <v>16</v>
       </c>
-      <c r="V18" s="171"/>
+      <c r="V18" s="187"/>
       <c r="AB18" s="3"/>
-      <c r="AC18" s="140" t="s">
+      <c r="AC18" s="158" t="s">
         <v>31</v>
       </c>
-      <c r="AD18" s="141"/>
-      <c r="AE18" s="140" t="s">
+      <c r="AD18" s="159"/>
+      <c r="AE18" s="158" t="s">
         <v>6</v>
       </c>
-      <c r="AF18" s="141"/>
-      <c r="AG18" s="140" t="s">
+      <c r="AF18" s="159"/>
+      <c r="AG18" s="158" t="s">
         <v>32</v>
       </c>
-      <c r="AH18" s="141"/>
-      <c r="AI18" s="140" t="s">
+      <c r="AH18" s="159"/>
+      <c r="AI18" s="158" t="s">
         <v>9</v>
       </c>
-      <c r="AJ18" s="141"/>
-      <c r="BC18" s="133" t="s">
+      <c r="AJ18" s="159"/>
+      <c r="BC18" s="129" t="s">
+        <v>82</v>
+      </c>
+      <c r="BD18" s="127"/>
+      <c r="BE18" s="129" t="s">
         <v>84</v>
       </c>
-      <c r="BD18" s="131"/>
-      <c r="BE18" s="133" t="s">
-        <v>86</v>
-      </c>
-      <c r="BF18" s="132"/>
-      <c r="BG18" s="131" t="s">
+      <c r="BF18" s="128"/>
+      <c r="BG18" s="127" t="s">
+        <v>83</v>
+      </c>
+      <c r="BH18" s="128"/>
+      <c r="BI18" s="129" t="s">
+        <v>82</v>
+      </c>
+      <c r="BJ18" s="127"/>
+      <c r="BK18" s="129" t="s">
+        <v>84</v>
+      </c>
+      <c r="BL18" s="128"/>
+      <c r="BM18" s="127" t="s">
+        <v>83</v>
+      </c>
+      <c r="BN18" s="128"/>
+      <c r="BO18" s="129" t="s">
         <v>85</v>
       </c>
-      <c r="BH18" s="132"/>
-      <c r="BI18" s="133" t="s">
+      <c r="BP18" s="127"/>
+      <c r="BQ18" s="129" t="s">
         <v>84</v>
       </c>
-      <c r="BJ18" s="131"/>
-      <c r="BK18" s="133" t="s">
-        <v>86</v>
-      </c>
-      <c r="BL18" s="132"/>
-      <c r="BM18" s="131" t="s">
+      <c r="BR18" s="128"/>
+      <c r="BS18" s="127" t="s">
+        <v>83</v>
+      </c>
+      <c r="BT18" s="128"/>
+      <c r="BU18" s="129" t="s">
         <v>85</v>
       </c>
-      <c r="BN18" s="132"/>
-      <c r="BO18" s="133" t="s">
-        <v>87</v>
-      </c>
-      <c r="BP18" s="131"/>
-      <c r="BQ18" s="133" t="s">
-        <v>86</v>
-      </c>
-      <c r="BR18" s="132"/>
-      <c r="BS18" s="131" t="s">
+      <c r="BV18" s="127"/>
+      <c r="BW18" s="129" t="s">
+        <v>84</v>
+      </c>
+      <c r="BX18" s="128"/>
+      <c r="BY18" s="127" t="s">
+        <v>83</v>
+      </c>
+      <c r="BZ18" s="128"/>
+      <c r="CD18" s="148" t="s">
+        <v>82</v>
+      </c>
+      <c r="CE18" s="149"/>
+      <c r="CF18" s="148" t="s">
+        <v>84</v>
+      </c>
+      <c r="CG18" s="149"/>
+      <c r="CH18" s="203" t="s">
+        <v>83</v>
+      </c>
+      <c r="CI18" s="149"/>
+      <c r="CJ18" s="148" t="s">
+        <v>82</v>
+      </c>
+      <c r="CK18" s="203"/>
+      <c r="CL18" s="148" t="s">
+        <v>84</v>
+      </c>
+      <c r="CM18" s="149"/>
+      <c r="CN18" s="203" t="s">
+        <v>83</v>
+      </c>
+      <c r="CO18" s="149"/>
+      <c r="CP18" s="148" t="s">
         <v>85</v>
       </c>
-      <c r="BT18" s="132"/>
-      <c r="BU18" s="133" t="s">
-        <v>87</v>
-      </c>
-      <c r="BV18" s="131"/>
-      <c r="BW18" s="133" t="s">
-        <v>86</v>
-      </c>
-      <c r="BX18" s="132"/>
-      <c r="BY18" s="131" t="s">
+      <c r="CQ18" s="203"/>
+      <c r="CR18" s="148" t="s">
+        <v>84</v>
+      </c>
+      <c r="CS18" s="149"/>
+      <c r="CT18" s="203" t="s">
+        <v>83</v>
+      </c>
+      <c r="CU18" s="149"/>
+      <c r="CV18" s="148" t="s">
         <v>85</v>
       </c>
-      <c r="BZ18" s="132"/>
-      <c r="CD18" s="197" t="s">
+      <c r="CW18" s="203"/>
+      <c r="CX18" s="148" t="s">
         <v>84</v>
       </c>
-      <c r="CE18" s="199"/>
-      <c r="CF18" s="197" t="s">
-        <v>86</v>
-      </c>
-      <c r="CG18" s="199"/>
-      <c r="CH18" s="198" t="s">
-        <v>85</v>
-      </c>
-      <c r="CI18" s="199"/>
-      <c r="CJ18" s="197" t="s">
-        <v>84</v>
-      </c>
-      <c r="CK18" s="198"/>
-      <c r="CL18" s="197" t="s">
-        <v>86</v>
-      </c>
-      <c r="CM18" s="199"/>
-      <c r="CN18" s="198" t="s">
-        <v>85</v>
-      </c>
-      <c r="CO18" s="199"/>
-      <c r="CP18" s="197" t="s">
-        <v>87</v>
-      </c>
-      <c r="CQ18" s="198"/>
-      <c r="CR18" s="197" t="s">
-        <v>86</v>
-      </c>
-      <c r="CS18" s="199"/>
-      <c r="CT18" s="198" t="s">
-        <v>85</v>
-      </c>
-      <c r="CU18" s="199"/>
-      <c r="CV18" s="197" t="s">
-        <v>87</v>
-      </c>
-      <c r="CW18" s="198"/>
-      <c r="CX18" s="197" t="s">
-        <v>86</v>
-      </c>
-      <c r="CY18" s="199"/>
-      <c r="CZ18" s="198" t="s">
-        <v>85</v>
-      </c>
-      <c r="DA18" s="199"/>
+      <c r="CY18" s="149"/>
+      <c r="CZ18" s="203" t="s">
+        <v>83</v>
+      </c>
+      <c r="DA18" s="149"/>
     </row>
     <row r="19" spans="1:105" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
@@ -4078,22 +4177,22 @@
       <c r="AB19" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="AC19" s="142" t="s">
+      <c r="AC19" s="160" t="s">
         <v>47</v>
       </c>
-      <c r="AD19" s="143"/>
-      <c r="AE19" s="142" t="s">
+      <c r="AD19" s="161"/>
+      <c r="AE19" s="160" t="s">
         <v>47</v>
       </c>
-      <c r="AF19" s="143"/>
-      <c r="AG19" s="142" t="s">
+      <c r="AF19" s="161"/>
+      <c r="AG19" s="160" t="s">
         <v>47</v>
       </c>
-      <c r="AH19" s="143"/>
-      <c r="AI19" s="142" t="s">
+      <c r="AH19" s="161"/>
+      <c r="AI19" s="160" t="s">
         <v>47</v>
       </c>
-      <c r="AJ19" s="143"/>
+      <c r="AJ19" s="161"/>
       <c r="BB19" s="2" t="s">
         <v>0</v>
       </c>
@@ -4172,54 +4271,54 @@
       <c r="CC19" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="CD19" s="200" t="s">
+      <c r="CD19" s="204" t="s">
         <v>45</v>
       </c>
-      <c r="CE19" s="184"/>
-      <c r="CF19" s="200" t="s">
+      <c r="CE19" s="198"/>
+      <c r="CF19" s="204" t="s">
         <v>45</v>
       </c>
-      <c r="CG19" s="184"/>
-      <c r="CH19" s="183" t="s">
+      <c r="CG19" s="198"/>
+      <c r="CH19" s="197" t="s">
         <v>45</v>
       </c>
-      <c r="CI19" s="184"/>
-      <c r="CJ19" s="200" t="s">
+      <c r="CI19" s="198"/>
+      <c r="CJ19" s="204" t="s">
         <v>45</v>
       </c>
-      <c r="CK19" s="183"/>
-      <c r="CL19" s="200" t="s">
+      <c r="CK19" s="197"/>
+      <c r="CL19" s="204" t="s">
         <v>45</v>
       </c>
-      <c r="CM19" s="184"/>
-      <c r="CN19" s="183" t="s">
+      <c r="CM19" s="198"/>
+      <c r="CN19" s="197" t="s">
         <v>45</v>
       </c>
-      <c r="CO19" s="184"/>
-      <c r="CP19" s="200" t="s">
+      <c r="CO19" s="198"/>
+      <c r="CP19" s="204" t="s">
         <v>45</v>
       </c>
-      <c r="CQ19" s="183"/>
-      <c r="CR19" s="200" t="s">
+      <c r="CQ19" s="197"/>
+      <c r="CR19" s="204" t="s">
         <v>45</v>
       </c>
-      <c r="CS19" s="184"/>
-      <c r="CT19" s="183" t="s">
+      <c r="CS19" s="198"/>
+      <c r="CT19" s="197" t="s">
         <v>45</v>
       </c>
-      <c r="CU19" s="184"/>
-      <c r="CV19" s="200" t="s">
+      <c r="CU19" s="198"/>
+      <c r="CV19" s="204" t="s">
         <v>45</v>
       </c>
-      <c r="CW19" s="183"/>
-      <c r="CX19" s="200" t="s">
+      <c r="CW19" s="197"/>
+      <c r="CX19" s="204" t="s">
         <v>45</v>
       </c>
-      <c r="CY19" s="184"/>
-      <c r="CZ19" s="183" t="s">
+      <c r="CY19" s="198"/>
+      <c r="CZ19" s="197" t="s">
         <v>45</v>
       </c>
-      <c r="DA19" s="184"/>
+      <c r="DA19" s="198"/>
     </row>
     <row r="20" spans="1:105" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
@@ -4292,26 +4391,26 @@
       <c r="AB20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AC20" s="137">
+      <c r="AC20" s="155">
         <f t="shared" ref="AC20:AC26" si="15">AVERAGE(B20:C20)</f>
         <v>0.89666666666666672</v>
       </c>
-      <c r="AD20" s="138"/>
-      <c r="AE20" s="137">
+      <c r="AD20" s="156"/>
+      <c r="AE20" s="155">
         <f t="shared" ref="AE20:AE26" si="16">AVERAGE(D20:E20)</f>
         <v>0.89999999999999991</v>
       </c>
-      <c r="AF20" s="138"/>
-      <c r="AG20" s="137">
+      <c r="AF20" s="156"/>
+      <c r="AG20" s="155">
         <f t="shared" ref="AG20:AG26" si="17">AVERAGE(F20:G20)</f>
         <v>0.89500000000000002</v>
       </c>
-      <c r="AH20" s="138"/>
-      <c r="AI20" s="137">
+      <c r="AH20" s="156"/>
+      <c r="AI20" s="155">
         <f t="shared" ref="AI20:AI26" si="18">AVERAGE(H20:I20)</f>
         <v>0.91500000000000004</v>
       </c>
-      <c r="AJ20" s="138"/>
+      <c r="AJ20" s="156"/>
       <c r="BB20" s="2" t="s">
         <v>1</v>
       </c>
@@ -4414,66 +4513,66 @@
       <c r="CC20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="CD20" s="187">
+      <c r="CD20" s="133">
         <f>AVERAGE(BC20:BD20)</f>
         <v>0.92</v>
       </c>
-      <c r="CE20" s="186"/>
-      <c r="CF20" s="187">
+      <c r="CE20" s="134"/>
+      <c r="CF20" s="133">
         <f>AVERAGE(BE20:BF20)</f>
         <v>0.93</v>
       </c>
-      <c r="CG20" s="186"/>
-      <c r="CH20" s="185">
+      <c r="CG20" s="134"/>
+      <c r="CH20" s="199">
         <f>AVERAGE(BG20:BH20)</f>
         <v>0.90500000000000003</v>
       </c>
-      <c r="CI20" s="186"/>
-      <c r="CJ20" s="187">
+      <c r="CI20" s="134"/>
+      <c r="CJ20" s="133">
         <f>AVERAGE(BI20:BJ20)</f>
         <v>0.87</v>
       </c>
-      <c r="CK20" s="185"/>
-      <c r="CL20" s="187">
+      <c r="CK20" s="199"/>
+      <c r="CL20" s="133">
         <f>AVERAGE(BK20:BL20)</f>
         <v>0.86749999999999994</v>
       </c>
-      <c r="CM20" s="186"/>
-      <c r="CN20" s="185">
+      <c r="CM20" s="134"/>
+      <c r="CN20" s="199">
         <f>AVERAGE(BM20:BN20)</f>
         <v>0.87749999999999995</v>
       </c>
-      <c r="CO20" s="186"/>
-      <c r="CP20" s="187">
+      <c r="CO20" s="134"/>
+      <c r="CP20" s="133">
         <f>AVERAGE(BO20:BP20)</f>
         <v>0.91</v>
       </c>
-      <c r="CQ20" s="185"/>
-      <c r="CR20" s="187">
+      <c r="CQ20" s="199"/>
+      <c r="CR20" s="133">
         <f>AVERAGE(BQ20:BR20)</f>
         <v>0.91</v>
       </c>
-      <c r="CS20" s="186"/>
-      <c r="CT20" s="185">
+      <c r="CS20" s="134"/>
+      <c r="CT20" s="199">
         <f>AVERAGE(BS20:BT20)</f>
         <v>0.91500000000000004</v>
       </c>
-      <c r="CU20" s="186"/>
-      <c r="CV20" s="187">
+      <c r="CU20" s="134"/>
+      <c r="CV20" s="133">
         <f>AVERAGE(BU20:BV20)</f>
         <v>0.8683333333333334</v>
       </c>
-      <c r="CW20" s="185"/>
-      <c r="CX20" s="187">
+      <c r="CW20" s="199"/>
+      <c r="CX20" s="133">
         <f>AVERAGE(BW20:BX20)</f>
         <v>0.875</v>
       </c>
-      <c r="CY20" s="186"/>
-      <c r="CZ20" s="185">
+      <c r="CY20" s="134"/>
+      <c r="CZ20" s="199">
         <f>AVERAGE(BY20:BZ20)</f>
         <v>0.87666666666666671</v>
       </c>
-      <c r="DA20" s="186"/>
+      <c r="DA20" s="134"/>
     </row>
     <row r="21" spans="1:105" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
@@ -4547,26 +4646,26 @@
       <c r="AB21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AC21" s="137">
+      <c r="AC21" s="155">
         <f t="shared" si="15"/>
         <v>0.14833333333333334</v>
       </c>
-      <c r="AD21" s="138"/>
-      <c r="AE21" s="137">
+      <c r="AD21" s="156"/>
+      <c r="AE21" s="155">
         <f t="shared" si="16"/>
         <v>0.17333333333333334</v>
       </c>
-      <c r="AF21" s="138"/>
-      <c r="AG21" s="137">
+      <c r="AF21" s="156"/>
+      <c r="AG21" s="155">
         <f t="shared" si="17"/>
         <v>0.16</v>
       </c>
-      <c r="AH21" s="138"/>
-      <c r="AI21" s="137">
+      <c r="AH21" s="156"/>
+      <c r="AI21" s="155">
         <f t="shared" si="18"/>
         <v>0.23333333333333334</v>
       </c>
-      <c r="AJ21" s="138"/>
+      <c r="AJ21" s="156"/>
       <c r="BB21" s="2" t="s">
         <v>2</v>
       </c>
@@ -4669,66 +4768,66 @@
       <c r="CC21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="CD21" s="187">
+      <c r="CD21" s="133">
         <f>AVERAGE(BC21:BD21)</f>
         <v>0.26500000000000001</v>
       </c>
-      <c r="CE21" s="186"/>
-      <c r="CF21" s="187">
+      <c r="CE21" s="134"/>
+      <c r="CF21" s="133">
         <f>AVERAGE(BE21:BF21)</f>
         <v>0.33750000000000002</v>
       </c>
-      <c r="CG21" s="186"/>
-      <c r="CH21" s="185">
+      <c r="CG21" s="134"/>
+      <c r="CH21" s="199">
         <f>AVERAGE(BG21:BH21)</f>
         <v>0.27250000000000002</v>
       </c>
-      <c r="CI21" s="186"/>
-      <c r="CJ21" s="187">
+      <c r="CI21" s="134"/>
+      <c r="CJ21" s="133">
         <f>AVERAGE(BI21:BJ21)</f>
         <v>0.15000000000000002</v>
       </c>
-      <c r="CK21" s="185"/>
-      <c r="CL21" s="187">
+      <c r="CK21" s="199"/>
+      <c r="CL21" s="133">
         <f>AVERAGE(BK21:BL21)</f>
         <v>0.23500000000000001</v>
       </c>
-      <c r="CM21" s="186"/>
-      <c r="CN21" s="185">
+      <c r="CM21" s="134"/>
+      <c r="CN21" s="199">
         <f>AVERAGE(BM21:BN21)</f>
         <v>0.19500000000000001</v>
       </c>
-      <c r="CO21" s="186"/>
-      <c r="CP21" s="187">
+      <c r="CO21" s="134"/>
+      <c r="CP21" s="133">
         <f>AVERAGE(BO21:BP21)</f>
         <v>0.27250000000000002</v>
       </c>
-      <c r="CQ21" s="185"/>
-      <c r="CR21" s="187">
+      <c r="CQ21" s="199"/>
+      <c r="CR21" s="133">
         <f>AVERAGE(BQ21:BR21)</f>
         <v>0.25</v>
       </c>
-      <c r="CS21" s="186"/>
-      <c r="CT21" s="185">
+      <c r="CS21" s="134"/>
+      <c r="CT21" s="199">
         <f>AVERAGE(BS21:BT21)</f>
         <v>0.27</v>
       </c>
-      <c r="CU21" s="186"/>
-      <c r="CV21" s="187">
+      <c r="CU21" s="134"/>
+      <c r="CV21" s="133">
         <f>AVERAGE(BU21:BV21)</f>
         <v>0.34666666666666668</v>
       </c>
-      <c r="CW21" s="185"/>
-      <c r="CX21" s="187">
+      <c r="CW21" s="199"/>
+      <c r="CX21" s="133">
         <f>AVERAGE(BW21:BX21)</f>
         <v>0.27500000000000002</v>
       </c>
-      <c r="CY21" s="186"/>
-      <c r="CZ21" s="185">
+      <c r="CY21" s="134"/>
+      <c r="CZ21" s="199">
         <f>AVERAGE(BY21:BZ21)</f>
         <v>0.32666666666666666</v>
       </c>
-      <c r="DA21" s="186"/>
+      <c r="DA21" s="134"/>
     </row>
     <row r="22" spans="1:105" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
@@ -4802,26 +4901,26 @@
       <c r="AB22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AC22" s="137">
+      <c r="AC22" s="155">
         <f t="shared" si="15"/>
         <v>0.32333333333333336</v>
       </c>
-      <c r="AD22" s="138"/>
-      <c r="AE22" s="137">
+      <c r="AD22" s="156"/>
+      <c r="AE22" s="155">
         <f t="shared" si="16"/>
         <v>0.29833333333333334</v>
       </c>
-      <c r="AF22" s="138"/>
-      <c r="AG22" s="137">
+      <c r="AF22" s="156"/>
+      <c r="AG22" s="155">
         <f t="shared" si="17"/>
         <v>0.22500000000000001</v>
       </c>
-      <c r="AH22" s="138"/>
-      <c r="AI22" s="137">
+      <c r="AH22" s="156"/>
+      <c r="AI22" s="155">
         <f t="shared" si="18"/>
         <v>0.19500000000000001</v>
       </c>
-      <c r="AJ22" s="138"/>
+      <c r="AJ22" s="156"/>
       <c r="BB22" s="2" t="s">
         <v>3</v>
       </c>
@@ -4924,66 +5023,66 @@
       <c r="CC22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="CD22" s="187">
+      <c r="CD22" s="133">
         <f>AVERAGE(BC22:BD22)</f>
         <v>6.25E-2</v>
       </c>
-      <c r="CE22" s="186"/>
-      <c r="CF22" s="187">
+      <c r="CE22" s="134"/>
+      <c r="CF22" s="133">
         <f>AVERAGE(BE22:BF22)</f>
         <v>7.5000000000000011E-2</v>
       </c>
-      <c r="CG22" s="186"/>
-      <c r="CH22" s="185">
+      <c r="CG22" s="134"/>
+      <c r="CH22" s="199">
         <f>AVERAGE(BG22:BH22)</f>
         <v>8.249999999999999E-2</v>
       </c>
-      <c r="CI22" s="186"/>
-      <c r="CJ22" s="187">
+      <c r="CI22" s="134"/>
+      <c r="CJ22" s="133">
         <f>AVERAGE(BI22:BJ22)</f>
         <v>0.32750000000000001</v>
       </c>
-      <c r="CK22" s="185"/>
-      <c r="CL22" s="187">
+      <c r="CK22" s="199"/>
+      <c r="CL22" s="133">
         <f>AVERAGE(BK22:BL22)</f>
         <v>0.33749999999999997</v>
       </c>
-      <c r="CM22" s="186"/>
-      <c r="CN22" s="185">
+      <c r="CM22" s="134"/>
+      <c r="CN22" s="199">
         <f>AVERAGE(BM22:BN22)</f>
         <v>0.3725</v>
       </c>
-      <c r="CO22" s="186"/>
-      <c r="CP22" s="187">
+      <c r="CO22" s="134"/>
+      <c r="CP22" s="133">
         <f>AVERAGE(BO22:BP22)</f>
         <v>0.54249999999999998</v>
       </c>
-      <c r="CQ22" s="185"/>
-      <c r="CR22" s="187">
+      <c r="CQ22" s="199"/>
+      <c r="CR22" s="133">
         <f>AVERAGE(BQ22:BR22)</f>
         <v>0.43500000000000005</v>
       </c>
-      <c r="CS22" s="186"/>
-      <c r="CT22" s="185">
+      <c r="CS22" s="134"/>
+      <c r="CT22" s="199">
         <f>AVERAGE(BS22:BT22)</f>
         <v>0.46249999999999997</v>
       </c>
-      <c r="CU22" s="186"/>
-      <c r="CV22" s="187">
+      <c r="CU22" s="134"/>
+      <c r="CV22" s="133">
         <f>AVERAGE(BU22:BV22)</f>
         <v>0.28666666666666668</v>
       </c>
-      <c r="CW22" s="185"/>
-      <c r="CX22" s="187">
+      <c r="CW22" s="199"/>
+      <c r="CX22" s="133">
         <f>AVERAGE(BW22:BX22)</f>
         <v>0.255</v>
       </c>
-      <c r="CY22" s="186"/>
-      <c r="CZ22" s="185">
+      <c r="CY22" s="134"/>
+      <c r="CZ22" s="199">
         <f>AVERAGE(BY22:BZ22)</f>
         <v>0.30666666666666664</v>
       </c>
-      <c r="DA22" s="186"/>
+      <c r="DA22" s="134"/>
     </row>
     <row r="23" spans="1:105" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
@@ -5057,26 +5156,26 @@
       <c r="AB23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AC23" s="137">
+      <c r="AC23" s="155">
         <f t="shared" si="15"/>
         <v>0.12666666666666668</v>
       </c>
-      <c r="AD23" s="138"/>
-      <c r="AE23" s="137">
+      <c r="AD23" s="156"/>
+      <c r="AE23" s="155">
         <f t="shared" si="16"/>
         <v>0.11499999999999999</v>
       </c>
-      <c r="AF23" s="138"/>
-      <c r="AG23" s="137">
+      <c r="AF23" s="156"/>
+      <c r="AG23" s="155">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="AH23" s="138"/>
-      <c r="AI23" s="137">
+      <c r="AH23" s="156"/>
+      <c r="AI23" s="155">
         <f t="shared" si="18"/>
         <v>9.1666666666666674E-2</v>
       </c>
-      <c r="AJ23" s="138"/>
+      <c r="AJ23" s="156"/>
       <c r="BB23" s="2" t="s">
         <v>4</v>
       </c>
@@ -5179,66 +5278,66 @@
       <c r="CC23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="CD23" s="204">
+      <c r="CD23" s="135">
         <f>AVERAGE(BC23:BD23)</f>
         <v>0.14249999999999999</v>
       </c>
-      <c r="CE23" s="181"/>
-      <c r="CF23" s="204">
+      <c r="CE23" s="136"/>
+      <c r="CF23" s="135">
         <f>AVERAGE(BE23:BF23)</f>
         <v>0.11749999999999999</v>
       </c>
-      <c r="CG23" s="181"/>
-      <c r="CH23" s="180">
+      <c r="CG23" s="136"/>
+      <c r="CH23" s="196">
         <f>AVERAGE(BG23:BH23)</f>
         <v>0.1875</v>
       </c>
-      <c r="CI23" s="181"/>
-      <c r="CJ23" s="204">
+      <c r="CI23" s="136"/>
+      <c r="CJ23" s="135">
         <f>AVERAGE(BI23:BJ23)</f>
         <v>0.10750000000000001</v>
       </c>
-      <c r="CK23" s="180"/>
-      <c r="CL23" s="204">
+      <c r="CK23" s="196"/>
+      <c r="CL23" s="135">
         <f>AVERAGE(BK23:BL23)</f>
         <v>0.11</v>
       </c>
-      <c r="CM23" s="181"/>
-      <c r="CN23" s="180">
+      <c r="CM23" s="136"/>
+      <c r="CN23" s="196">
         <f>AVERAGE(BM23:BN23)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="CO23" s="181"/>
-      <c r="CP23" s="204">
+      <c r="CO23" s="136"/>
+      <c r="CP23" s="135">
         <f>AVERAGE(BO23:BP23)</f>
         <v>0.22999999999999998</v>
       </c>
-      <c r="CQ23" s="180"/>
-      <c r="CR23" s="204">
+      <c r="CQ23" s="196"/>
+      <c r="CR23" s="135">
         <f>AVERAGE(BQ23:BR23)</f>
         <v>0.20499999999999999</v>
       </c>
-      <c r="CS23" s="181"/>
-      <c r="CT23" s="180">
+      <c r="CS23" s="136"/>
+      <c r="CT23" s="196">
         <f>AVERAGE(BS23:BT23)</f>
         <v>0.28749999999999998</v>
       </c>
-      <c r="CU23" s="181"/>
-      <c r="CV23" s="204">
+      <c r="CU23" s="136"/>
+      <c r="CV23" s="135">
         <f>AVERAGE(BU23:BV23)</f>
         <v>0.17499999999999999</v>
       </c>
-      <c r="CW23" s="180"/>
-      <c r="CX23" s="204">
+      <c r="CW23" s="196"/>
+      <c r="CX23" s="135">
         <f>AVERAGE(BW23:BX23)</f>
         <v>0.11</v>
       </c>
-      <c r="CY23" s="181"/>
-      <c r="CZ23" s="180">
+      <c r="CY23" s="136"/>
+      <c r="CZ23" s="196">
         <f>AVERAGE(BY23:BZ23)</f>
         <v>0.17833333333333334</v>
       </c>
-      <c r="DA23" s="181"/>
+      <c r="DA23" s="136"/>
     </row>
     <row r="24" spans="1:105" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
@@ -5316,26 +5415,26 @@
       <c r="AB24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AC24" s="144">
+      <c r="AC24" s="162">
         <f t="shared" si="15"/>
         <v>0.79166666666666674</v>
       </c>
-      <c r="AD24" s="145"/>
-      <c r="AE24" s="144">
+      <c r="AD24" s="163"/>
+      <c r="AE24" s="162">
         <f t="shared" si="16"/>
         <v>0.79500000000000004</v>
       </c>
-      <c r="AF24" s="145"/>
-      <c r="AG24" s="144">
+      <c r="AF24" s="163"/>
+      <c r="AG24" s="162">
         <f t="shared" si="17"/>
         <v>0.79</v>
       </c>
-      <c r="AH24" s="145"/>
-      <c r="AI24" s="144">
+      <c r="AH24" s="163"/>
+      <c r="AI24" s="162">
         <f t="shared" si="18"/>
         <v>0.81833333333333336</v>
       </c>
-      <c r="AJ24" s="145"/>
+      <c r="AJ24" s="163"/>
       <c r="BB24" s="2" t="s">
         <v>5</v>
       </c>
@@ -5438,66 +5537,66 @@
       <c r="CC24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="CD24" s="188">
+      <c r="CD24" s="200">
         <f>AVERAGE(BC24:BD24)</f>
         <v>0.82</v>
       </c>
-      <c r="CE24" s="190"/>
-      <c r="CF24" s="188">
+      <c r="CE24" s="202"/>
+      <c r="CF24" s="200">
         <f>AVERAGE(BE24:BF24)</f>
         <v>0.84</v>
       </c>
-      <c r="CG24" s="190"/>
-      <c r="CH24" s="189">
+      <c r="CG24" s="202"/>
+      <c r="CH24" s="201">
         <f>AVERAGE(BG24:BH24)</f>
         <v>0.80500000000000005</v>
       </c>
-      <c r="CI24" s="190"/>
-      <c r="CJ24" s="188">
+      <c r="CI24" s="202"/>
+      <c r="CJ24" s="200">
         <f>AVERAGE(BI24:BJ24)</f>
         <v>0.73</v>
       </c>
-      <c r="CK24" s="189"/>
-      <c r="CL24" s="188">
+      <c r="CK24" s="201"/>
+      <c r="CL24" s="200">
         <f>AVERAGE(BK24:BL24)</f>
         <v>0.73</v>
       </c>
-      <c r="CM24" s="190"/>
-      <c r="CN24" s="189">
+      <c r="CM24" s="202"/>
+      <c r="CN24" s="201">
         <f>AVERAGE(BM24:BN24)</f>
         <v>0.73750000000000004</v>
       </c>
-      <c r="CO24" s="190"/>
-      <c r="CP24" s="188">
+      <c r="CO24" s="202"/>
+      <c r="CP24" s="200">
         <f>AVERAGE(BO24:BP24)</f>
         <v>0.81500000000000006</v>
       </c>
-      <c r="CQ24" s="189"/>
-      <c r="CR24" s="188">
+      <c r="CQ24" s="201"/>
+      <c r="CR24" s="200">
         <f>AVERAGE(BQ24:BR24)</f>
         <v>0.8</v>
       </c>
-      <c r="CS24" s="190"/>
-      <c r="CT24" s="189">
+      <c r="CS24" s="202"/>
+      <c r="CT24" s="201">
         <f>AVERAGE(BS24:BT24)</f>
         <v>0.8125</v>
       </c>
-      <c r="CU24" s="190"/>
-      <c r="CV24" s="188">
+      <c r="CU24" s="202"/>
+      <c r="CV24" s="200">
         <f>AVERAGE(BU24:BV24)</f>
         <v>0.74666666666666659</v>
       </c>
-      <c r="CW24" s="189"/>
-      <c r="CX24" s="188">
+      <c r="CW24" s="201"/>
+      <c r="CX24" s="200">
         <f>AVERAGE(BW24:BX24)</f>
         <v>0.74</v>
       </c>
-      <c r="CY24" s="190"/>
-      <c r="CZ24" s="189">
+      <c r="CY24" s="202"/>
+      <c r="CZ24" s="201">
         <f>AVERAGE(BY24:BZ24)</f>
         <v>0.76333333333333342</v>
       </c>
-      <c r="DA24" s="190"/>
+      <c r="DA24" s="202"/>
     </row>
     <row r="25" spans="1:105" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
@@ -5556,39 +5655,39 @@
         <v>325</v>
       </c>
       <c r="R25" s="9"/>
-      <c r="S25" s="169">
+      <c r="S25" s="185">
         <f>SUM(S24:T24)</f>
         <v>1295</v>
       </c>
-      <c r="T25" s="169"/>
-      <c r="U25" s="172">
+      <c r="T25" s="185"/>
+      <c r="U25" s="188">
         <f>SUM(U24:V24)</f>
         <v>1295</v>
       </c>
-      <c r="V25" s="172"/>
+      <c r="V25" s="188"/>
       <c r="AB25" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AC25" s="148">
+      <c r="AC25" s="137">
         <f>AVERAGE(AC20:AD23)</f>
         <v>0.37375000000000008</v>
       </c>
-      <c r="AD25" s="149"/>
-      <c r="AE25" s="148">
+      <c r="AD25" s="138"/>
+      <c r="AE25" s="137">
         <f>AVERAGE(AE20:AF23)</f>
         <v>0.37166666666666665</v>
       </c>
-      <c r="AF25" s="149"/>
-      <c r="AG25" s="148">
+      <c r="AF25" s="138"/>
+      <c r="AG25" s="137">
         <f>AVERAGE(AG20:AH23)</f>
         <v>0.32</v>
       </c>
-      <c r="AH25" s="149"/>
-      <c r="AI25" s="148">
+      <c r="AH25" s="138"/>
+      <c r="AI25" s="137">
         <f>AVERAGE(AI20:AJ23)</f>
         <v>0.35875000000000001</v>
       </c>
-      <c r="AJ25" s="149"/>
+      <c r="AJ25" s="138"/>
       <c r="BB25" s="2" t="s">
         <v>43</v>
       </c>
@@ -5691,66 +5790,66 @@
       <c r="CC25" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="CD25" s="148">
+      <c r="CD25" s="137">
         <f>AVERAGE(CD20:CE23)</f>
         <v>0.34750000000000003</v>
       </c>
-      <c r="CE25" s="149"/>
-      <c r="CF25" s="182">
+      <c r="CE25" s="138"/>
+      <c r="CF25" s="139">
         <f>AVERAGE(CF20:CG23)</f>
         <v>0.36499999999999999</v>
       </c>
-      <c r="CG25" s="149"/>
-      <c r="CH25" s="182">
+      <c r="CG25" s="138"/>
+      <c r="CH25" s="139">
         <f>AVERAGE(CH20:CI23)</f>
         <v>0.361875</v>
       </c>
-      <c r="CI25" s="149"/>
-      <c r="CJ25" s="182">
+      <c r="CI25" s="138"/>
+      <c r="CJ25" s="139">
         <f>AVERAGE(CJ20:CK23)</f>
         <v>0.36375000000000002</v>
       </c>
-      <c r="CK25" s="149"/>
-      <c r="CL25" s="182">
+      <c r="CK25" s="138"/>
+      <c r="CL25" s="139">
         <f>AVERAGE(CL20:CM23)</f>
         <v>0.38750000000000001</v>
       </c>
-      <c r="CM25" s="149"/>
-      <c r="CN25" s="182">
+      <c r="CM25" s="138"/>
+      <c r="CN25" s="139">
         <f>AVERAGE(CN20:CO23)</f>
         <v>0.37812500000000004</v>
       </c>
-      <c r="CO25" s="149"/>
-      <c r="CP25" s="182">
+      <c r="CO25" s="138"/>
+      <c r="CP25" s="139">
         <f>AVERAGE(CP20:CQ23)</f>
         <v>0.48875000000000002</v>
       </c>
-      <c r="CQ25" s="149"/>
-      <c r="CR25" s="182">
+      <c r="CQ25" s="138"/>
+      <c r="CR25" s="139">
         <f>AVERAGE(CR20:CS23)</f>
         <v>0.45000000000000007</v>
       </c>
-      <c r="CS25" s="149"/>
-      <c r="CT25" s="182">
+      <c r="CS25" s="138"/>
+      <c r="CT25" s="139">
         <f>AVERAGE(CT20:CU23)</f>
         <v>0.48375000000000001</v>
       </c>
-      <c r="CU25" s="149"/>
-      <c r="CV25" s="182">
+      <c r="CU25" s="138"/>
+      <c r="CV25" s="139">
         <f>AVERAGE(CV20:CW23)</f>
         <v>0.41916666666666669</v>
       </c>
-      <c r="CW25" s="149"/>
-      <c r="CX25" s="182">
+      <c r="CW25" s="138"/>
+      <c r="CX25" s="139">
         <f>AVERAGE(CX20:CY23)</f>
         <v>0.37874999999999998</v>
       </c>
-      <c r="CY25" s="149"/>
-      <c r="CZ25" s="182">
+      <c r="CY25" s="138"/>
+      <c r="CZ25" s="139">
         <f>AVERAGE(CZ20:DA23)</f>
         <v>0.42208333333333337</v>
       </c>
-      <c r="DA25" s="149"/>
+      <c r="DA25" s="138"/>
     </row>
     <row r="26" spans="1:105" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
@@ -5789,39 +5888,39 @@
         <v>0.78666666666666674</v>
       </c>
       <c r="K26" s="9"/>
-      <c r="L26" s="169">
+      <c r="L26" s="185">
         <f>SUM(L25:M25)</f>
         <v>1295</v>
       </c>
-      <c r="M26" s="169"/>
-      <c r="N26" s="172">
+      <c r="M26" s="185"/>
+      <c r="N26" s="188">
         <f>SUM(N25:O25)</f>
         <v>1295</v>
       </c>
-      <c r="O26" s="172"/>
+      <c r="O26" s="188"/>
       <c r="AB26" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AC26" s="134">
+      <c r="AC26" s="150">
         <f t="shared" si="15"/>
         <v>0.77499999999999991</v>
       </c>
-      <c r="AD26" s="135"/>
-      <c r="AE26" s="134">
+      <c r="AD26" s="151"/>
+      <c r="AE26" s="150">
         <f t="shared" si="16"/>
         <v>0.77666666666666662</v>
       </c>
-      <c r="AF26" s="135"/>
-      <c r="AG26" s="134">
+      <c r="AF26" s="151"/>
+      <c r="AG26" s="150">
         <f t="shared" si="17"/>
         <v>0.76500000000000001</v>
       </c>
-      <c r="AH26" s="135"/>
-      <c r="AI26" s="134">
+      <c r="AH26" s="151"/>
+      <c r="AI26" s="150">
         <f t="shared" si="18"/>
         <v>0.78833333333333333</v>
       </c>
-      <c r="AJ26" s="135"/>
+      <c r="AJ26" s="151"/>
       <c r="BB26" s="2" t="s">
         <v>44</v>
       </c>
@@ -5924,66 +6023,66 @@
       <c r="CC26" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="CD26" s="134">
+      <c r="CD26" s="150">
         <f>AVERAGE(BC26:BD26)</f>
         <v>0.87749999999999995</v>
       </c>
-      <c r="CE26" s="135"/>
-      <c r="CF26" s="134">
+      <c r="CE26" s="151"/>
+      <c r="CF26" s="150">
         <f>AVERAGE(BE26:BF26)</f>
         <v>0.88749999999999996</v>
       </c>
-      <c r="CG26" s="135"/>
+      <c r="CG26" s="151"/>
       <c r="CH26" s="205">
         <f>AVERAGE(BG26:BH26)</f>
         <v>0.86499999999999999</v>
       </c>
-      <c r="CI26" s="135"/>
-      <c r="CJ26" s="134">
+      <c r="CI26" s="151"/>
+      <c r="CJ26" s="150">
         <f>AVERAGE(BI26:BJ26)</f>
         <v>0.7</v>
       </c>
       <c r="CK26" s="205"/>
-      <c r="CL26" s="134">
+      <c r="CL26" s="150">
         <f>AVERAGE(BK26:BL26)</f>
         <v>0.7024999999999999</v>
       </c>
-      <c r="CM26" s="135"/>
+      <c r="CM26" s="151"/>
       <c r="CN26" s="205">
         <f>AVERAGE(BM26:BN26)</f>
         <v>0.71</v>
       </c>
-      <c r="CO26" s="135"/>
-      <c r="CP26" s="134">
+      <c r="CO26" s="151"/>
+      <c r="CP26" s="150">
         <f>AVERAGE(BO26:BP26)</f>
         <v>0.8274999999999999</v>
       </c>
       <c r="CQ26" s="205"/>
-      <c r="CR26" s="134">
+      <c r="CR26" s="150">
         <f>AVERAGE(BQ26:BR26)</f>
         <v>0.8125</v>
       </c>
-      <c r="CS26" s="135"/>
+      <c r="CS26" s="151"/>
       <c r="CT26" s="205">
         <f>AVERAGE(BS26:BT26)</f>
         <v>0.82499999999999996</v>
       </c>
-      <c r="CU26" s="135"/>
-      <c r="CV26" s="134">
+      <c r="CU26" s="151"/>
+      <c r="CV26" s="150">
         <f>AVERAGE(BU26:BV26)</f>
         <v>0.77333333333333343</v>
       </c>
       <c r="CW26" s="205"/>
-      <c r="CX26" s="134">
+      <c r="CX26" s="150">
         <f>AVERAGE(BW26:BX26)</f>
         <v>0.76500000000000001</v>
       </c>
-      <c r="CY26" s="135"/>
+      <c r="CY26" s="151"/>
       <c r="CZ26" s="205">
         <f>AVERAGE(BY26:BZ26)</f>
         <v>0.77666666666666662</v>
       </c>
-      <c r="DA26" s="135"/>
+      <c r="DA26" s="151"/>
     </row>
     <row r="27" spans="1:105" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
@@ -6000,62 +6099,62 @@
       <c r="E29" s="1"/>
     </row>
     <row r="31" spans="1:105" ht="26" x14ac:dyDescent="0.6">
-      <c r="A31" s="164" t="s">
+      <c r="A31" s="180" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="164"/>
-      <c r="C31" s="164"/>
-      <c r="D31" s="164"/>
-      <c r="E31" s="164"/>
-      <c r="F31" s="164"/>
-      <c r="G31" s="164"/>
-      <c r="H31" s="164"/>
-      <c r="I31" s="164"/>
-      <c r="J31" s="164"/>
-      <c r="K31" s="164"/>
-      <c r="L31" s="164"/>
-      <c r="M31" s="164"/>
-      <c r="N31" s="164"/>
-      <c r="O31" s="164"/>
-      <c r="P31" s="164"/>
-      <c r="Q31" s="164"/>
-      <c r="R31" s="164"/>
-      <c r="S31" s="164"/>
-      <c r="T31" s="164"/>
-      <c r="U31" s="164"/>
+      <c r="B31" s="180"/>
+      <c r="C31" s="180"/>
+      <c r="D31" s="180"/>
+      <c r="E31" s="180"/>
+      <c r="F31" s="180"/>
+      <c r="G31" s="180"/>
+      <c r="H31" s="180"/>
+      <c r="I31" s="180"/>
+      <c r="J31" s="180"/>
+      <c r="K31" s="180"/>
+      <c r="L31" s="180"/>
+      <c r="M31" s="180"/>
+      <c r="N31" s="180"/>
+      <c r="O31" s="180"/>
+      <c r="P31" s="180"/>
+      <c r="Q31" s="180"/>
+      <c r="R31" s="180"/>
+      <c r="S31" s="180"/>
+      <c r="T31" s="180"/>
+      <c r="U31" s="180"/>
       <c r="BB31" s="113"/>
-      <c r="BC31" s="136" t="s">
+      <c r="BC31" s="143" t="s">
         <v>10</v>
       </c>
-      <c r="BD31" s="123"/>
-      <c r="BE31" s="123" t="s">
+      <c r="BD31" s="144"/>
+      <c r="BE31" s="144" t="s">
         <v>11</v>
       </c>
-      <c r="BF31" s="124"/>
-      <c r="BI31" s="136" t="s">
+      <c r="BF31" s="145"/>
+      <c r="BI31" s="143" t="s">
         <v>10</v>
       </c>
-      <c r="BJ31" s="123"/>
-      <c r="BK31" s="123" t="s">
+      <c r="BJ31" s="144"/>
+      <c r="BK31" s="144" t="s">
         <v>11</v>
       </c>
-      <c r="BL31" s="124"/>
-      <c r="BO31" s="136" t="s">
+      <c r="BL31" s="145"/>
+      <c r="BO31" s="143" t="s">
         <v>10</v>
       </c>
-      <c r="BP31" s="123"/>
-      <c r="BQ31" s="123" t="s">
+      <c r="BP31" s="144"/>
+      <c r="BQ31" s="144" t="s">
         <v>11</v>
       </c>
-      <c r="BR31" s="124"/>
-      <c r="BU31" s="136" t="s">
+      <c r="BR31" s="145"/>
+      <c r="BU31" s="143" t="s">
         <v>10</v>
       </c>
-      <c r="BV31" s="123"/>
-      <c r="BW31" s="123" t="s">
+      <c r="BV31" s="144"/>
+      <c r="BW31" s="144" t="s">
         <v>11</v>
       </c>
-      <c r="BX31" s="124"/>
+      <c r="BX31" s="145"/>
     </row>
     <row r="32" spans="1:105" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="BB32" s="114"/>
@@ -6107,31 +6206,31 @@
       <c r="BX32" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="CM32" s="129" t="s">
+      <c r="CM32" s="125" t="s">
+        <v>82</v>
+      </c>
+      <c r="CN32" s="125"/>
+      <c r="CO32" s="125" t="s">
         <v>84</v>
       </c>
-      <c r="CN32" s="129"/>
-      <c r="CO32" s="129" t="s">
-        <v>86</v>
-      </c>
-      <c r="CP32" s="129"/>
-      <c r="CQ32" s="129" t="s">
-        <v>85</v>
-      </c>
-      <c r="CR32" s="129"/>
+      <c r="CP32" s="125"/>
+      <c r="CQ32" s="125" t="s">
+        <v>83</v>
+      </c>
+      <c r="CR32" s="125"/>
     </row>
     <row r="33" spans="1:101" ht="26" x14ac:dyDescent="0.6">
-      <c r="A33" s="176" t="s">
+      <c r="A33" s="192" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="176"/>
-      <c r="C33" s="176"/>
-      <c r="D33" s="176"/>
-      <c r="E33" s="176"/>
-      <c r="F33" s="176"/>
+      <c r="B33" s="192"/>
+      <c r="C33" s="192"/>
+      <c r="D33" s="192"/>
+      <c r="E33" s="192"/>
+      <c r="F33" s="192"/>
       <c r="L33" s="17"/>
       <c r="M33" s="91" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="N33" s="91"/>
       <c r="O33" s="91"/>
@@ -6202,22 +6301,22 @@
         <v>262</v>
       </c>
       <c r="CM33" s="109" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="CN33" s="110" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="CO33" s="109" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="CP33" s="108" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="CQ33" s="110" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="CR33" s="108" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="CW33" s="122"/>
     </row>
@@ -6701,14 +6800,14 @@
       </c>
     </row>
     <row r="38" spans="1:101" ht="26" x14ac:dyDescent="0.6">
-      <c r="A38" s="176" t="s">
+      <c r="A38" s="192" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="176"/>
-      <c r="C38" s="176"/>
-      <c r="D38" s="176"/>
-      <c r="E38" s="176"/>
-      <c r="F38" s="176"/>
+      <c r="B38" s="192"/>
+      <c r="C38" s="192"/>
+      <c r="D38" s="192"/>
+      <c r="E38" s="192"/>
+      <c r="F38" s="192"/>
       <c r="H38" s="11" t="s">
         <v>21</v>
       </c>
@@ -6856,58 +6955,58 @@
         <v>30</v>
       </c>
       <c r="J39" s="15"/>
-      <c r="K39" s="167"/>
-      <c r="L39" s="167"/>
-      <c r="M39" s="168"/>
-      <c r="N39" s="168"/>
+      <c r="K39" s="183"/>
+      <c r="L39" s="183"/>
+      <c r="M39" s="184"/>
+      <c r="N39" s="184"/>
       <c r="O39" s="15"/>
       <c r="P39" s="15"/>
       <c r="Q39" s="16"/>
-      <c r="R39" s="167"/>
-      <c r="S39" s="167"/>
-      <c r="T39" s="168"/>
-      <c r="U39" s="168"/>
+      <c r="R39" s="183"/>
+      <c r="S39" s="183"/>
+      <c r="T39" s="184"/>
+      <c r="U39" s="184"/>
       <c r="BB39" s="115"/>
-      <c r="BC39" s="125">
+      <c r="BC39" s="146">
         <f>SUM(BC38:BD38)</f>
         <v>1295</v>
       </c>
-      <c r="BD39" s="126"/>
-      <c r="BE39" s="127">
+      <c r="BD39" s="147"/>
+      <c r="BE39" s="123">
         <f>SUM(BE38:BF38)</f>
         <v>1295</v>
       </c>
-      <c r="BF39" s="128"/>
-      <c r="BI39" s="125">
+      <c r="BF39" s="124"/>
+      <c r="BI39" s="146">
         <f>SUM(BI38:BJ38)</f>
         <v>1295</v>
       </c>
-      <c r="BJ39" s="126"/>
-      <c r="BK39" s="127">
+      <c r="BJ39" s="147"/>
+      <c r="BK39" s="123">
         <f>SUM(BK38:BL38)</f>
         <v>1295</v>
       </c>
-      <c r="BL39" s="128"/>
-      <c r="BO39" s="125">
+      <c r="BL39" s="124"/>
+      <c r="BO39" s="146">
         <f>SUM(BO38:BP38)</f>
         <v>1295</v>
       </c>
-      <c r="BP39" s="126"/>
-      <c r="BQ39" s="127">
+      <c r="BP39" s="147"/>
+      <c r="BQ39" s="123">
         <f>SUM(BQ38:BR38)</f>
         <v>1295</v>
       </c>
-      <c r="BR39" s="128"/>
-      <c r="BU39" s="125">
+      <c r="BR39" s="124"/>
+      <c r="BU39" s="146">
         <f>SUM(BU38:BV38)</f>
         <v>1295</v>
       </c>
-      <c r="BV39" s="126"/>
-      <c r="BW39" s="127">
+      <c r="BV39" s="147"/>
+      <c r="BW39" s="123">
         <f>SUM(BW38:BX38)</f>
         <v>1295</v>
       </c>
-      <c r="BX39" s="128"/>
+      <c r="BX39" s="124"/>
       <c r="CL39" s="2" t="s">
         <v>43</v>
       </c>
@@ -6984,14 +7083,14 @@
       </c>
     </row>
     <row r="43" spans="1:101" ht="26" x14ac:dyDescent="0.6">
-      <c r="A43" s="176" t="s">
+      <c r="A43" s="192" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="176"/>
-      <c r="C43" s="176"/>
-      <c r="D43" s="176"/>
-      <c r="E43" s="176"/>
-      <c r="F43" s="176"/>
+      <c r="B43" s="192"/>
+      <c r="C43" s="192"/>
+      <c r="D43" s="192"/>
+      <c r="E43" s="192"/>
+      <c r="F43" s="192"/>
     </row>
     <row r="44" spans="1:101" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="28" t="s">
@@ -7033,69 +7132,116 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A49" s="30"/>
     </row>
-    <row r="50" spans="1:21" ht="26" x14ac:dyDescent="0.6">
-      <c r="A50" s="164" t="s">
+    <row r="50" spans="1:43" ht="26" x14ac:dyDescent="0.6">
+      <c r="A50" s="180" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" s="180"/>
+      <c r="C50" s="180"/>
+      <c r="D50" s="180"/>
+      <c r="E50" s="180"/>
+      <c r="F50" s="180"/>
+      <c r="G50" s="180"/>
+      <c r="H50" s="180"/>
+      <c r="I50" s="180"/>
+      <c r="J50" s="180"/>
+      <c r="K50" s="180"/>
+      <c r="L50" s="180"/>
+      <c r="M50" s="180"/>
+      <c r="N50" s="180"/>
+      <c r="O50" s="180"/>
+      <c r="P50" s="180"/>
+      <c r="Q50" s="180"/>
+      <c r="R50" s="180"/>
+      <c r="S50" s="180"/>
+      <c r="T50" s="180"/>
+      <c r="U50" s="180"/>
+      <c r="W50" s="180" t="s">
+        <v>89</v>
+      </c>
+      <c r="X50" s="180"/>
+      <c r="Y50" s="180"/>
+      <c r="Z50" s="180"/>
+      <c r="AA50" s="180"/>
+      <c r="AB50" s="180"/>
+      <c r="AC50" s="180"/>
+      <c r="AD50" s="180"/>
+      <c r="AE50" s="180"/>
+      <c r="AF50" s="180"/>
+      <c r="AG50" s="180"/>
+      <c r="AH50" s="180"/>
+      <c r="AI50" s="180"/>
+      <c r="AJ50" s="180"/>
+      <c r="AK50" s="180"/>
+      <c r="AL50" s="180"/>
+      <c r="AM50" s="180"/>
+      <c r="AN50" s="180"/>
+      <c r="AO50" s="180"/>
+      <c r="AP50" s="180"/>
+      <c r="AQ50" s="180"/>
+    </row>
+    <row r="52" spans="1:43" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="181" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="193"/>
+      <c r="D52" s="181" t="s">
+        <v>33</v>
+      </c>
+      <c r="E52" s="182"/>
+      <c r="F52" s="193" t="s">
+        <v>49</v>
+      </c>
+      <c r="G52" s="182"/>
+      <c r="H52" s="194" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="164"/>
-      <c r="C50" s="164"/>
-      <c r="D50" s="164"/>
-      <c r="E50" s="164"/>
-      <c r="F50" s="164"/>
-      <c r="G50" s="164"/>
-      <c r="H50" s="164"/>
-      <c r="I50" s="164"/>
-      <c r="J50" s="164"/>
-      <c r="K50" s="164"/>
-      <c r="L50" s="164"/>
-      <c r="M50" s="164"/>
-      <c r="N50" s="164"/>
-      <c r="O50" s="164"/>
-      <c r="P50" s="164"/>
-      <c r="Q50" s="164"/>
-      <c r="R50" s="164"/>
-      <c r="S50" s="164"/>
-      <c r="T50" s="164"/>
-      <c r="U50" s="164"/>
+      <c r="I52" s="195"/>
+      <c r="L52" s="174" t="s">
+        <v>6</v>
+      </c>
+      <c r="M52" s="175"/>
+      <c r="N52" s="174" t="s">
+        <v>33</v>
+      </c>
+      <c r="O52" s="175"/>
+      <c r="P52" s="174" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q52" s="175"/>
+      <c r="R52" s="174" t="s">
+        <v>55</v>
+      </c>
+      <c r="S52" s="175"/>
+      <c r="W52" s="194" t="s">
+        <v>90</v>
+      </c>
+      <c r="X52" s="195"/>
+      <c r="Y52" s="194" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z52" s="195"/>
+      <c r="AA52" s="194" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB52" s="195"/>
+      <c r="AF52" s="174" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG52" s="175"/>
+      <c r="AH52" s="174" t="s">
+        <v>92</v>
+      </c>
+      <c r="AI52" s="175"/>
+      <c r="AJ52" s="174" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK52" s="175"/>
     </row>
-    <row r="52" spans="1:21" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="165" t="s">
-        <v>6</v>
-      </c>
-      <c r="C52" s="177"/>
-      <c r="D52" s="165" t="s">
-        <v>33</v>
-      </c>
-      <c r="E52" s="166"/>
-      <c r="F52" s="177" t="s">
-        <v>49</v>
-      </c>
-      <c r="G52" s="166"/>
-      <c r="H52" s="178" t="s">
-        <v>57</v>
-      </c>
-      <c r="I52" s="179"/>
-      <c r="L52" s="158" t="s">
-        <v>6</v>
-      </c>
-      <c r="M52" s="159"/>
-      <c r="N52" s="158" t="s">
-        <v>33</v>
-      </c>
-      <c r="O52" s="159"/>
-      <c r="P52" s="158" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q52" s="159"/>
-      <c r="R52" s="158" t="s">
-        <v>57</v>
-      </c>
-      <c r="S52" s="159"/>
-    </row>
-    <row r="53" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:43" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53" s="36" t="s">
         <v>0</v>
       </c>
@@ -7126,24 +7272,60 @@
       <c r="K53" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="L53" s="160" t="s">
+      <c r="L53" s="176" t="s">
         <v>53</v>
       </c>
-      <c r="M53" s="161"/>
-      <c r="N53" s="160" t="s">
+      <c r="M53" s="177"/>
+      <c r="N53" s="176" t="s">
         <v>53</v>
       </c>
-      <c r="O53" s="161"/>
-      <c r="P53" s="160" t="s">
+      <c r="O53" s="177"/>
+      <c r="P53" s="176" t="s">
         <v>53</v>
       </c>
-      <c r="Q53" s="161"/>
-      <c r="R53" s="160" t="s">
+      <c r="Q53" s="177"/>
+      <c r="R53" s="176" t="s">
         <v>53</v>
       </c>
-      <c r="S53" s="161"/>
+      <c r="S53" s="177"/>
+      <c r="V53" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="W53" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="X53" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y53" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z53" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA53" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB53" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE53" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF53" s="176" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG53" s="177"/>
+      <c r="AH53" s="176" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI53" s="177"/>
+      <c r="AJ53" s="176" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK53" s="177"/>
     </row>
-    <row r="54" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:43" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A54" s="36" t="s">
         <v>17</v>
       </c>
@@ -7182,28 +7364,73 @@
       <c r="K54" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="L54" s="162">
+      <c r="L54" s="178">
         <f t="shared" ref="L54:L59" si="28">AVERAGE(B54:C54)</f>
         <v>0.94999999999999984</v>
       </c>
-      <c r="M54" s="163"/>
-      <c r="N54" s="162">
+      <c r="M54" s="179"/>
+      <c r="N54" s="178">
         <f t="shared" ref="N54:N56" si="29">AVERAGE(D54:E54)</f>
         <v>0.94333333333333336</v>
       </c>
-      <c r="O54" s="163"/>
-      <c r="P54" s="162">
+      <c r="O54" s="179"/>
+      <c r="P54" s="178">
         <f t="shared" ref="P54:P59" si="30">AVERAGE(F54:G54)</f>
         <v>0.94999999999999984</v>
       </c>
-      <c r="Q54" s="163"/>
-      <c r="R54" s="162">
+      <c r="Q54" s="179"/>
+      <c r="R54" s="178">
         <f t="shared" ref="R54:R59" si="31">AVERAGE(H54:I54)</f>
         <v>0.92500000000000004</v>
       </c>
-      <c r="S54" s="163"/>
+      <c r="S54" s="179"/>
+      <c r="V54" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="W54" s="62">
+        <f>AVERAGE(0.94, 0.94       )</f>
+        <v>0.94</v>
+      </c>
+      <c r="X54" s="64">
+        <f>AVERAGE(0.95, 0.95       )</f>
+        <v>0.95</v>
+      </c>
+      <c r="Y54" s="62">
+        <f>AVERAGE(0.88, 0.88       )</f>
+        <v>0.88</v>
+      </c>
+      <c r="Z54" s="63">
+        <f>AVERAGE(0.88, 0.88       )</f>
+        <v>0.88</v>
+      </c>
+      <c r="AA54" s="64">
+        <f>AVERAGE(0.95, 0.94       )</f>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="AB54" s="63">
+        <f>AVERAGE(0.95, 0.94       )</f>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="AE54" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF54" s="178">
+        <f>AVERAGE(W54:X54)</f>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="AG54" s="179"/>
+      <c r="AH54" s="178">
+        <f t="shared" ref="AH54:AH59" si="32">AVERAGE(Y54:Z54)</f>
+        <v>0.88</v>
+      </c>
+      <c r="AI54" s="179"/>
+      <c r="AJ54" s="178">
+        <f t="shared" ref="AJ54:AJ59" si="33">AVERAGE(AA54:AB54)</f>
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="AK54" s="179"/>
     </row>
-    <row r="55" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:43" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A55" s="36" t="s">
         <v>18</v>
       </c>
@@ -7242,28 +7469,73 @@
       <c r="K55" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="L55" s="162">
+      <c r="L55" s="178">
         <f t="shared" si="28"/>
         <v>0.50166666666666671</v>
       </c>
-      <c r="M55" s="163"/>
-      <c r="N55" s="162">
+      <c r="M55" s="179"/>
+      <c r="N55" s="178">
         <f t="shared" si="29"/>
         <v>0.48833333333333334</v>
       </c>
-      <c r="O55" s="163"/>
-      <c r="P55" s="162">
+      <c r="O55" s="179"/>
+      <c r="P55" s="178">
         <f t="shared" si="30"/>
         <v>0.54</v>
       </c>
-      <c r="Q55" s="163"/>
-      <c r="R55" s="162">
+      <c r="Q55" s="179"/>
+      <c r="R55" s="178">
         <f t="shared" si="31"/>
         <v>0.41000000000000003</v>
       </c>
-      <c r="S55" s="163"/>
+      <c r="S55" s="179"/>
+      <c r="V55" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="W55" s="62">
+        <f>AVERAGE(0, 0        )</f>
+        <v>0</v>
+      </c>
+      <c r="X55" s="64">
+        <f>AVERAGE(0, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y55" s="62">
+        <f>AVERAGE(0.34, 0.23        )</f>
+        <v>0.28500000000000003</v>
+      </c>
+      <c r="Z55" s="63">
+        <f>AVERAGE(0.32, 0.24        )</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AA55" s="64">
+        <f>AVERAGE(0.34, 0.32        )</f>
+        <v>0.33</v>
+      </c>
+      <c r="AB55" s="63">
+        <f>AVERAGE(0.36, 0.33        )</f>
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="AE55" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF55" s="178">
+        <f t="shared" ref="AF55:AF59" si="34">AVERAGE(W55:X55)</f>
+        <v>0</v>
+      </c>
+      <c r="AG55" s="179"/>
+      <c r="AH55" s="178">
+        <f t="shared" si="32"/>
+        <v>0.28250000000000003</v>
+      </c>
+      <c r="AI55" s="179"/>
+      <c r="AJ55" s="178">
+        <f t="shared" si="33"/>
+        <v>0.33750000000000002</v>
+      </c>
+      <c r="AK55" s="179"/>
     </row>
-    <row r="56" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:43" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A56" s="36" t="s">
         <v>19</v>
       </c>
@@ -7302,28 +7574,73 @@
       <c r="K56" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="L56" s="150">
+      <c r="L56" s="166">
         <f t="shared" si="28"/>
         <v>0.99499999999999988</v>
       </c>
-      <c r="M56" s="151"/>
-      <c r="N56" s="150">
+      <c r="M56" s="167"/>
+      <c r="N56" s="166">
         <f t="shared" si="29"/>
         <v>0.99499999999999988</v>
       </c>
-      <c r="O56" s="151"/>
-      <c r="P56" s="150">
+      <c r="O56" s="167"/>
+      <c r="P56" s="166">
         <f t="shared" si="30"/>
         <v>0.99499999999999988</v>
       </c>
-      <c r="Q56" s="151"/>
-      <c r="R56" s="150">
+      <c r="Q56" s="167"/>
+      <c r="R56" s="166">
         <f t="shared" si="31"/>
         <v>0.995</v>
       </c>
-      <c r="S56" s="151"/>
+      <c r="S56" s="167"/>
+      <c r="V56" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="W56" s="62">
+        <f>AVERAGE(0.99, 0.99        )</f>
+        <v>0.99</v>
+      </c>
+      <c r="X56" s="64">
+        <f>AVERAGE(1, 1        )</f>
+        <v>1</v>
+      </c>
+      <c r="Y56" s="62">
+        <f>AVERAGE(0, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z56" s="63">
+        <f>AVERAGE(0, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA56" s="64">
+        <f>AVERAGE(0.99, 0.99        )</f>
+        <v>0.99</v>
+      </c>
+      <c r="AB56" s="63">
+        <f>AVERAGE(1, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="AE56" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF56" s="178">
+        <f t="shared" si="34"/>
+        <v>0.995</v>
+      </c>
+      <c r="AG56" s="179"/>
+      <c r="AH56" s="178">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="AI56" s="179"/>
+      <c r="AJ56" s="178">
+        <f t="shared" si="33"/>
+        <v>0.995</v>
+      </c>
+      <c r="AK56" s="179"/>
     </row>
-    <row r="57" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:43" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A57" s="36" t="s">
         <v>5</v>
       </c>
@@ -7362,88 +7679,178 @@
       <c r="K57" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="L57" s="152">
+      <c r="L57" s="168">
         <f t="shared" si="28"/>
         <v>0.91833333333333333</v>
       </c>
-      <c r="M57" s="153"/>
-      <c r="N57" s="152">
+      <c r="M57" s="169"/>
+      <c r="N57" s="168">
         <f>AVERAGE(D57:E57)</f>
         <v>0.90666666666666673</v>
       </c>
-      <c r="O57" s="153"/>
-      <c r="P57" s="152">
+      <c r="O57" s="169"/>
+      <c r="P57" s="168">
         <f t="shared" si="30"/>
         <v>0.91833333333333333</v>
       </c>
-      <c r="Q57" s="153"/>
-      <c r="R57" s="152">
+      <c r="Q57" s="169"/>
+      <c r="R57" s="168">
         <f t="shared" si="31"/>
         <v>0.88500000000000001</v>
       </c>
-      <c r="S57" s="153"/>
+      <c r="S57" s="169"/>
+      <c r="V57" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="W57" s="206">
+        <f>AVERAGE(0.9, 0.9       )</f>
+        <v>0.9</v>
+      </c>
+      <c r="X57" s="207">
+        <f>AVERAGE(0.91, 0.91       )</f>
+        <v>0.91</v>
+      </c>
+      <c r="Y57" s="206">
+        <f>AVERAGE(0.78, 0.78       )</f>
+        <v>0.78</v>
+      </c>
+      <c r="Z57" s="208">
+        <f>AVERAGE(0.78, 0.78)</f>
+        <v>0.78</v>
+      </c>
+      <c r="AA57" s="207">
+        <f>AVERAGE(0.91, 0.9       )</f>
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="AB57" s="208">
+        <f>AVERAGE(0.92, 0.91       )</f>
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="AE57" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF57" s="209">
+        <f t="shared" si="34"/>
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="AG57" s="210"/>
+      <c r="AH57" s="209">
+        <f t="shared" si="32"/>
+        <v>0.78</v>
+      </c>
+      <c r="AI57" s="210"/>
+      <c r="AJ57" s="209">
+        <f t="shared" si="33"/>
+        <v>0.91</v>
+      </c>
+      <c r="AK57" s="210"/>
     </row>
-    <row r="58" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:43" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A58" s="36" t="s">
         <v>52</v>
       </c>
       <c r="B58" s="71">
-        <f t="shared" ref="B58:I58" si="32">AVERAGE(B54:B56)</f>
+        <f t="shared" ref="B58:I58" si="35">AVERAGE(B54:B56)</f>
         <v>0.81555555555555548</v>
       </c>
       <c r="C58" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>0.81555555555555548</v>
       </c>
       <c r="D58" s="71">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>0.80888888888888888</v>
       </c>
       <c r="E58" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>0.80888888888888888</v>
       </c>
       <c r="F58" s="73">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>0.82777777777777761</v>
       </c>
       <c r="G58" s="73">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>0.82888888888888879</v>
       </c>
       <c r="H58" s="71">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>0.77833333333333332</v>
       </c>
       <c r="I58" s="72">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
         <v>0.77500000000000002</v>
       </c>
       <c r="K58" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="L58" s="154">
+      <c r="L58" s="170">
         <f t="shared" si="28"/>
         <v>0.81555555555555548</v>
       </c>
-      <c r="M58" s="155"/>
-      <c r="N58" s="154">
+      <c r="M58" s="171"/>
+      <c r="N58" s="170">
         <f>AVERAGE(D58:E58)</f>
         <v>0.80888888888888888</v>
       </c>
-      <c r="O58" s="155"/>
-      <c r="P58" s="154">
+      <c r="O58" s="171"/>
+      <c r="P58" s="170">
         <f t="shared" si="30"/>
         <v>0.82833333333333314</v>
       </c>
-      <c r="Q58" s="155"/>
-      <c r="R58" s="154">
+      <c r="Q58" s="171"/>
+      <c r="R58" s="170">
         <f t="shared" si="31"/>
         <v>0.77666666666666662</v>
       </c>
-      <c r="S58" s="155"/>
+      <c r="S58" s="171"/>
+      <c r="V58" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="W58" s="71">
+        <f>AVERAGE(0.64, 0.64       )</f>
+        <v>0.64</v>
+      </c>
+      <c r="X58" s="73">
+        <f>AVERAGE(0.65, 0.65       )</f>
+        <v>0.65</v>
+      </c>
+      <c r="Y58" s="71">
+        <f>AVERAGE(0.41, 0.37       )</f>
+        <v>0.39</v>
+      </c>
+      <c r="Z58" s="72">
+        <f>AVERAGE(0.4, 0.38)</f>
+        <v>0.39</v>
+      </c>
+      <c r="AA58" s="73">
+        <f>AVERAGE(0.76, 0.75       )</f>
+        <v>0.755</v>
+      </c>
+      <c r="AB58" s="72">
+        <f>AVERAGE(0.77, 0.76       )</f>
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="AE58" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF58" s="170">
+        <f>AVERAGE(AF54:AG56)</f>
+        <v>0.64666666666666661</v>
+      </c>
+      <c r="AG58" s="171"/>
+      <c r="AH58" s="170">
+        <f>AVERAGE(AH54:AI56)</f>
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="AI58" s="171"/>
+      <c r="AJ58" s="170">
+        <f>AVERAGE(AJ54:AK56)</f>
+        <v>0.75916666666666666</v>
+      </c>
+      <c r="AK58" s="171"/>
     </row>
-    <row r="59" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:43" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A59" s="36" t="s">
         <v>44</v>
       </c>
@@ -7482,28 +7889,73 @@
       <c r="K59" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="L59" s="156">
+      <c r="L59" s="172">
         <f t="shared" si="28"/>
         <v>0.91166666666666674</v>
       </c>
-      <c r="M59" s="157"/>
-      <c r="N59" s="156">
+      <c r="M59" s="173"/>
+      <c r="N59" s="172">
         <f>AVERAGE(D59:E59)</f>
         <v>0.90666666666666673</v>
       </c>
-      <c r="O59" s="157"/>
-      <c r="P59" s="156">
+      <c r="O59" s="173"/>
+      <c r="P59" s="172">
         <f t="shared" si="30"/>
         <v>0.91666666666666663</v>
       </c>
-      <c r="Q59" s="157"/>
-      <c r="R59" s="156">
+      <c r="Q59" s="173"/>
+      <c r="R59" s="172">
         <f t="shared" si="31"/>
         <v>0.88500000000000001</v>
       </c>
-      <c r="S59" s="157"/>
+      <c r="S59" s="173"/>
+      <c r="V59" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="W59" s="65">
+        <f>AVERAGE(0.86, 0.86       )</f>
+        <v>0.86</v>
+      </c>
+      <c r="X59" s="67">
+        <f>AVERAGE(0.87, 0.87       )</f>
+        <v>0.87</v>
+      </c>
+      <c r="Y59" s="65">
+        <f>AVERAGE(0.73, 0.72       )</f>
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="Z59" s="66">
+        <f>AVERAGE(0.72, 0.72)</f>
+        <v>0.72</v>
+      </c>
+      <c r="AA59" s="67">
+        <f>AVERAGE(0.89, 0.89       )</f>
+        <v>0.89</v>
+      </c>
+      <c r="AB59" s="66">
+        <f>AVERAGE(0.9, 0.9       )</f>
+        <v>0.9</v>
+      </c>
+      <c r="AE59" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF59" s="172">
+        <f t="shared" si="34"/>
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="AG59" s="173"/>
+      <c r="AH59" s="172">
+        <f t="shared" si="32"/>
+        <v>0.72249999999999992</v>
+      </c>
+      <c r="AI59" s="173"/>
+      <c r="AJ59" s="172">
+        <f t="shared" si="33"/>
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="AK59" s="173"/>
     </row>
-    <row r="60" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:43" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B60" s="34"/>
       <c r="C60" s="34"/>
       <c r="D60" s="34"/>
@@ -7513,7 +7965,7 @@
       <c r="H60" s="34"/>
       <c r="I60" s="34"/>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:43" x14ac:dyDescent="0.35">
       <c r="B61" s="35"/>
       <c r="C61" s="35"/>
       <c r="D61" s="35"/>
@@ -7523,68 +7975,68 @@
       <c r="H61" s="35"/>
       <c r="I61" s="35"/>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:43" x14ac:dyDescent="0.35">
       <c r="H62" s="35"/>
       <c r="I62" s="35"/>
     </row>
-    <row r="64" spans="1:21" ht="26" x14ac:dyDescent="0.6">
-      <c r="A64" s="164" t="s">
-        <v>54</v>
-      </c>
-      <c r="B64" s="164"/>
-      <c r="C64" s="164"/>
-      <c r="D64" s="164"/>
-      <c r="E64" s="164"/>
-      <c r="F64" s="164"/>
-      <c r="G64" s="164"/>
-      <c r="H64" s="164"/>
-      <c r="I64" s="164"/>
-      <c r="J64" s="164"/>
-      <c r="K64" s="164"/>
-      <c r="L64" s="164"/>
-      <c r="M64" s="164"/>
-      <c r="N64" s="164"/>
-      <c r="O64" s="164"/>
-      <c r="P64" s="164"/>
-      <c r="Q64" s="164"/>
-      <c r="R64" s="164"/>
-      <c r="S64" s="164"/>
-      <c r="T64" s="164"/>
-      <c r="U64" s="164"/>
+    <row r="64" spans="1:43" ht="26" x14ac:dyDescent="0.6">
+      <c r="A64" s="180" t="s">
+        <v>87</v>
+      </c>
+      <c r="B64" s="180"/>
+      <c r="C64" s="180"/>
+      <c r="D64" s="180"/>
+      <c r="E64" s="180"/>
+      <c r="F64" s="180"/>
+      <c r="G64" s="180"/>
+      <c r="H64" s="180"/>
+      <c r="I64" s="180"/>
+      <c r="J64" s="180"/>
+      <c r="K64" s="180"/>
+      <c r="L64" s="180"/>
+      <c r="M64" s="180"/>
+      <c r="N64" s="180"/>
+      <c r="O64" s="180"/>
+      <c r="P64" s="180"/>
+      <c r="Q64" s="180"/>
+      <c r="R64" s="180"/>
+      <c r="S64" s="180"/>
+      <c r="T64" s="180"/>
+      <c r="U64" s="180"/>
     </row>
     <row r="66" spans="1:19" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="165" t="s">
+      <c r="B66" s="181" t="s">
         <v>6</v>
       </c>
-      <c r="C66" s="166"/>
-      <c r="D66" s="165" t="s">
+      <c r="C66" s="182"/>
+      <c r="D66" s="181" t="s">
         <v>33</v>
       </c>
-      <c r="E66" s="166"/>
-      <c r="F66" s="165" t="s">
+      <c r="E66" s="182"/>
+      <c r="F66" s="181" t="s">
         <v>49</v>
       </c>
-      <c r="G66" s="166"/>
-      <c r="H66" s="165" t="s">
-        <v>57</v>
-      </c>
-      <c r="I66" s="166"/>
-      <c r="L66" s="158" t="s">
+      <c r="G66" s="182"/>
+      <c r="H66" s="181" t="s">
+        <v>55</v>
+      </c>
+      <c r="I66" s="182"/>
+      <c r="L66" s="174" t="s">
         <v>6</v>
       </c>
-      <c r="M66" s="159"/>
-      <c r="N66" s="158" t="s">
+      <c r="M66" s="175"/>
+      <c r="N66" s="174" t="s">
         <v>33</v>
       </c>
-      <c r="O66" s="159"/>
-      <c r="P66" s="158" t="s">
+      <c r="O66" s="175"/>
+      <c r="P66" s="174" t="s">
         <v>49</v>
       </c>
-      <c r="Q66" s="159"/>
-      <c r="R66" s="158" t="s">
-        <v>57</v>
-      </c>
-      <c r="S66" s="159"/>
+      <c r="Q66" s="175"/>
+      <c r="R66" s="174" t="s">
+        <v>55</v>
+      </c>
+      <c r="S66" s="175"/>
     </row>
     <row r="67" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A67" s="36" t="s">
@@ -7617,22 +8069,22 @@
       <c r="K67" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="L67" s="160" t="s">
+      <c r="L67" s="176" t="s">
         <v>53</v>
       </c>
-      <c r="M67" s="161"/>
-      <c r="N67" s="160" t="s">
+      <c r="M67" s="177"/>
+      <c r="N67" s="176" t="s">
         <v>53</v>
       </c>
-      <c r="O67" s="161"/>
-      <c r="P67" s="160" t="s">
+      <c r="O67" s="177"/>
+      <c r="P67" s="176" t="s">
         <v>53</v>
       </c>
-      <c r="Q67" s="161"/>
-      <c r="R67" s="160" t="s">
+      <c r="Q67" s="177"/>
+      <c r="R67" s="176" t="s">
         <v>53</v>
       </c>
-      <c r="S67" s="161"/>
+      <c r="S67" s="177"/>
     </row>
     <row r="68" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A68" s="36" t="s">
@@ -7673,26 +8125,26 @@
       <c r="K68" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="L68" s="162">
-        <f t="shared" ref="L68:L73" si="33">AVERAGE(B68:C68)</f>
+      <c r="L68" s="178">
+        <f t="shared" ref="L68:L73" si="36">AVERAGE(B68:C68)</f>
         <v>0.88666666666666671</v>
       </c>
-      <c r="M68" s="163"/>
-      <c r="N68" s="162">
-        <f t="shared" ref="N68:N73" si="34">AVERAGE(D68:E68)</f>
+      <c r="M68" s="179"/>
+      <c r="N68" s="178">
+        <f t="shared" ref="N68:N73" si="37">AVERAGE(D68:E68)</f>
         <v>0.87</v>
       </c>
-      <c r="O68" s="163"/>
-      <c r="P68" s="162">
-        <f t="shared" ref="P68:P73" si="35">AVERAGE(F68:G68)</f>
+      <c r="O68" s="179"/>
+      <c r="P68" s="178">
+        <f t="shared" ref="P68:P73" si="38">AVERAGE(F68:G68)</f>
         <v>0.87</v>
       </c>
-      <c r="Q68" s="163"/>
-      <c r="R68" s="162">
-        <f t="shared" ref="R68:R73" si="36">AVERAGE(H68:I68)</f>
+      <c r="Q68" s="179"/>
+      <c r="R68" s="178">
+        <f t="shared" ref="R68:R73" si="39">AVERAGE(H68:I68)</f>
         <v>0.87</v>
       </c>
-      <c r="S68" s="163"/>
+      <c r="S68" s="179"/>
     </row>
     <row r="69" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A69" s="36" t="s">
@@ -7733,26 +8185,26 @@
       <c r="K69" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="L69" s="162">
-        <f t="shared" si="33"/>
+      <c r="L69" s="178">
+        <f t="shared" si="36"/>
         <v>0.55833333333333335</v>
       </c>
-      <c r="M69" s="163"/>
-      <c r="N69" s="162">
-        <f t="shared" si="34"/>
+      <c r="M69" s="179"/>
+      <c r="N69" s="178">
+        <f t="shared" si="37"/>
         <v>0.42749999999999999</v>
       </c>
-      <c r="O69" s="163"/>
-      <c r="P69" s="162">
-        <f t="shared" si="35"/>
+      <c r="O69" s="179"/>
+      <c r="P69" s="178">
+        <f t="shared" si="38"/>
         <v>0.45999999999999996</v>
       </c>
-      <c r="Q69" s="163"/>
-      <c r="R69" s="162">
-        <f t="shared" si="36"/>
+      <c r="Q69" s="179"/>
+      <c r="R69" s="178">
+        <f t="shared" si="39"/>
         <v>0.38500000000000001</v>
       </c>
-      <c r="S69" s="163"/>
+      <c r="S69" s="179"/>
     </row>
     <row r="70" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A70" s="36" t="s">
@@ -7793,26 +8245,26 @@
       <c r="K70" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="L70" s="150">
-        <f t="shared" si="33"/>
+      <c r="L70" s="166">
+        <f t="shared" si="36"/>
         <v>0.15833333333333333</v>
       </c>
-      <c r="M70" s="151"/>
-      <c r="N70" s="150">
-        <f t="shared" si="34"/>
+      <c r="M70" s="167"/>
+      <c r="N70" s="166">
+        <f t="shared" si="37"/>
         <v>0.22999999999999998</v>
       </c>
-      <c r="O70" s="151"/>
-      <c r="P70" s="150">
-        <f t="shared" si="35"/>
+      <c r="O70" s="167"/>
+      <c r="P70" s="166">
+        <f t="shared" si="38"/>
         <v>0.215</v>
       </c>
-      <c r="Q70" s="151"/>
-      <c r="R70" s="150">
-        <f t="shared" si="36"/>
+      <c r="Q70" s="167"/>
+      <c r="R70" s="166">
+        <f t="shared" si="39"/>
         <v>0.27250000000000002</v>
       </c>
-      <c r="S70" s="151"/>
+      <c r="S70" s="167"/>
     </row>
     <row r="71" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A71" s="36" t="s">
@@ -7853,88 +8305,88 @@
       <c r="K71" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="L71" s="152">
-        <f t="shared" si="33"/>
+      <c r="L71" s="168">
+        <f t="shared" si="36"/>
         <v>0.79166666666666674</v>
       </c>
-      <c r="M71" s="153"/>
-      <c r="N71" s="152">
-        <f t="shared" si="34"/>
+      <c r="M71" s="169"/>
+      <c r="N71" s="168">
+        <f t="shared" si="37"/>
         <v>0.76249999999999996</v>
       </c>
-      <c r="O71" s="153"/>
-      <c r="P71" s="152">
-        <f t="shared" si="35"/>
+      <c r="O71" s="169"/>
+      <c r="P71" s="168">
+        <f t="shared" si="38"/>
         <v>0.76500000000000001</v>
       </c>
-      <c r="Q71" s="153"/>
-      <c r="R71" s="152">
-        <f t="shared" si="36"/>
+      <c r="Q71" s="169"/>
+      <c r="R71" s="168">
+        <f t="shared" si="39"/>
         <v>0.76500000000000001</v>
       </c>
-      <c r="S71" s="153"/>
+      <c r="S71" s="169"/>
     </row>
     <row r="72" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A72" s="36" t="s">
         <v>52</v>
       </c>
       <c r="B72" s="71">
-        <f t="shared" ref="B72:I72" si="37">AVERAGE(B68:B70)</f>
+        <f t="shared" ref="B72:I72" si="40">AVERAGE(B68:B70)</f>
         <v>0.52888888888888885</v>
       </c>
       <c r="C72" s="72">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>0.54</v>
       </c>
       <c r="D72" s="73">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>0.51166666666666671</v>
       </c>
       <c r="E72" s="73">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>0.50666666666666671</v>
       </c>
       <c r="F72" s="71">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>0.51500000000000001</v>
       </c>
       <c r="G72" s="72">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>0.51500000000000001</v>
       </c>
       <c r="H72" s="71">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>0.50833333333333341</v>
       </c>
       <c r="I72" s="72">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>0.51000000000000012</v>
       </c>
       <c r="K72" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="L72" s="154">
+      <c r="L72" s="170">
         <f>AVERAGE(B72:C72)</f>
         <v>0.5344444444444445</v>
       </c>
-      <c r="M72" s="155"/>
-      <c r="N72" s="154">
-        <f t="shared" si="34"/>
+      <c r="M72" s="171"/>
+      <c r="N72" s="170">
+        <f t="shared" si="37"/>
         <v>0.50916666666666677</v>
       </c>
-      <c r="O72" s="155"/>
-      <c r="P72" s="154">
-        <f t="shared" si="35"/>
+      <c r="O72" s="171"/>
+      <c r="P72" s="170">
+        <f t="shared" si="38"/>
         <v>0.51500000000000001</v>
       </c>
-      <c r="Q72" s="155"/>
-      <c r="R72" s="154">
-        <f t="shared" si="36"/>
+      <c r="Q72" s="171"/>
+      <c r="R72" s="170">
+        <f t="shared" si="39"/>
         <v>0.50916666666666677</v>
       </c>
-      <c r="S72" s="155"/>
+      <c r="S72" s="171"/>
     </row>
-    <row r="73" spans="1:19" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A73" s="36" t="s">
         <v>44</v>
       </c>
@@ -7973,47 +8425,47 @@
       <c r="K73" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="L73" s="156">
-        <f t="shared" si="33"/>
+      <c r="L73" s="172">
+        <f t="shared" si="36"/>
         <v>0.76833333333333331</v>
       </c>
-      <c r="M73" s="157"/>
-      <c r="N73" s="156">
-        <f t="shared" si="34"/>
+      <c r="M73" s="173"/>
+      <c r="N73" s="172">
+        <f t="shared" si="37"/>
         <v>0.75249999999999995</v>
       </c>
-      <c r="O73" s="157"/>
-      <c r="P73" s="156">
-        <f t="shared" si="35"/>
+      <c r="O73" s="173"/>
+      <c r="P73" s="172">
+        <f t="shared" si="38"/>
         <v>0.755</v>
       </c>
-      <c r="Q73" s="157"/>
-      <c r="R73" s="156">
-        <f t="shared" si="36"/>
+      <c r="Q73" s="173"/>
+      <c r="R73" s="172">
+        <f t="shared" si="39"/>
         <v>0.76</v>
       </c>
-      <c r="S73" s="157"/>
+      <c r="S73" s="173"/>
     </row>
     <row r="79" spans="1:19" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="40" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C81" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="D81" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="E81" s="41" t="s">
         <v>68</v>
-      </c>
-      <c r="D81" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="E81" s="41" t="s">
-        <v>70</v>
       </c>
       <c r="F81" s="41" t="s">
         <v>43</v>
       </c>
       <c r="G81" s="41" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H81" s="41" t="s">
         <v>5</v>
@@ -8021,7 +8473,7 @@
     </row>
     <row r="82" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C82" s="42">
         <v>70</v>
@@ -8045,7 +8497,7 @@
     </row>
     <row r="83" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C83" s="42">
         <v>70</v>
@@ -8069,7 +8521,7 @@
     </row>
     <row r="84" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C84" s="42">
         <v>70</v>
@@ -8081,7 +8533,7 @@
         <v>99</v>
       </c>
       <c r="F84" s="43">
-        <f t="shared" ref="F84:F90" si="38">AVERAGE(C84:E84)</f>
+        <f t="shared" ref="F84:F90" si="41">AVERAGE(C84:E84)</f>
         <v>62.666666666666664</v>
       </c>
       <c r="G84" s="42">
@@ -8093,7 +8545,7 @@
     </row>
     <row r="85" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C85" s="42">
         <v>73</v>
@@ -8105,7 +8557,7 @@
         <v>99</v>
       </c>
       <c r="F85" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>64.333333333333329</v>
       </c>
       <c r="G85" s="42">
@@ -8117,7 +8569,7 @@
     </row>
     <row r="86" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C86" s="42">
         <v>85</v>
@@ -8129,7 +8581,7 @@
         <v>99</v>
       </c>
       <c r="F86" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>68.333333333333329</v>
       </c>
       <c r="G86" s="42">
@@ -8141,7 +8593,7 @@
     </row>
     <row r="87" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C87" s="42">
         <v>92</v>
@@ -8153,7 +8605,7 @@
         <v>99</v>
       </c>
       <c r="F87" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>68</v>
       </c>
       <c r="G87" s="42">
@@ -8165,7 +8617,7 @@
     </row>
     <row r="88" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C88" s="42">
         <v>93</v>
@@ -8177,7 +8629,7 @@
         <v>99</v>
       </c>
       <c r="F88" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>69</v>
       </c>
       <c r="G88" s="42">
@@ -8189,7 +8641,7 @@
     </row>
     <row r="89" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C89" s="42">
         <v>93</v>
@@ -8201,7 +8653,7 @@
         <v>99</v>
       </c>
       <c r="F89" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>64</v>
       </c>
       <c r="G89" s="42">
@@ -8213,7 +8665,7 @@
     </row>
     <row r="90" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C90" s="42">
         <v>94</v>
@@ -8225,7 +8677,7 @@
         <v>99</v>
       </c>
       <c r="F90" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>64.333333333333329</v>
       </c>
       <c r="G90" s="42">
@@ -8236,7 +8688,33 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="426">
+  <mergeCells count="454">
+    <mergeCell ref="AF59:AG59"/>
+    <mergeCell ref="AH59:AI59"/>
+    <mergeCell ref="AJ59:AK59"/>
+    <mergeCell ref="AF56:AG56"/>
+    <mergeCell ref="AH56:AI56"/>
+    <mergeCell ref="AJ56:AK56"/>
+    <mergeCell ref="AF57:AG57"/>
+    <mergeCell ref="AH57:AI57"/>
+    <mergeCell ref="AJ57:AK57"/>
+    <mergeCell ref="AF58:AG58"/>
+    <mergeCell ref="AH58:AI58"/>
+    <mergeCell ref="AJ58:AK58"/>
+    <mergeCell ref="AF53:AG53"/>
+    <mergeCell ref="AH53:AI53"/>
+    <mergeCell ref="AJ53:AK53"/>
+    <mergeCell ref="AF54:AG54"/>
+    <mergeCell ref="AH54:AI54"/>
+    <mergeCell ref="AJ54:AK54"/>
+    <mergeCell ref="AF55:AG55"/>
+    <mergeCell ref="AH55:AI55"/>
+    <mergeCell ref="AJ55:AK55"/>
+    <mergeCell ref="AA52:AB52"/>
+    <mergeCell ref="W50:AQ50"/>
+    <mergeCell ref="AF52:AG52"/>
+    <mergeCell ref="AH52:AI52"/>
+    <mergeCell ref="AJ52:AK52"/>
     <mergeCell ref="CQ32:CR32"/>
     <mergeCell ref="CM32:CN32"/>
     <mergeCell ref="CH25:CI25"/>
@@ -8281,8 +8759,6 @@
     <mergeCell ref="CX22:CY22"/>
     <mergeCell ref="CZ22:DA22"/>
     <mergeCell ref="CH23:CI23"/>
-    <mergeCell ref="CD20:CE20"/>
-    <mergeCell ref="CD21:CE21"/>
     <mergeCell ref="CZ20:DA20"/>
     <mergeCell ref="CF21:CG21"/>
     <mergeCell ref="CH21:CI21"/>
@@ -8295,10 +8771,6 @@
     <mergeCell ref="CV21:CW21"/>
     <mergeCell ref="CX21:CY21"/>
     <mergeCell ref="CZ21:DA21"/>
-    <mergeCell ref="CF18:CG18"/>
-    <mergeCell ref="CH18:CI18"/>
-    <mergeCell ref="CJ18:CK18"/>
-    <mergeCell ref="CL18:CM18"/>
     <mergeCell ref="CN18:CO18"/>
     <mergeCell ref="CD19:CE19"/>
     <mergeCell ref="CF19:CG19"/>
@@ -8306,6 +8778,8 @@
     <mergeCell ref="CJ19:CK19"/>
     <mergeCell ref="CL19:CM19"/>
     <mergeCell ref="CN19:CO19"/>
+    <mergeCell ref="CD20:CE20"/>
+    <mergeCell ref="CD21:CE21"/>
     <mergeCell ref="CV17:DA17"/>
     <mergeCell ref="CP18:CQ18"/>
     <mergeCell ref="CR18:CS18"/>
@@ -8354,6 +8828,8 @@
     <mergeCell ref="N58:O58"/>
     <mergeCell ref="N59:O59"/>
     <mergeCell ref="L54:M54"/>
+    <mergeCell ref="W52:X52"/>
+    <mergeCell ref="Y52:Z52"/>
     <mergeCell ref="A43:F43"/>
     <mergeCell ref="A33:F33"/>
     <mergeCell ref="D4:E4"/>
@@ -8663,11 +9139,15 @@
     <mergeCell ref="CD17:CI17"/>
     <mergeCell ref="CJ17:CO17"/>
     <mergeCell ref="CD18:CE18"/>
+    <mergeCell ref="CF18:CG18"/>
+    <mergeCell ref="CH18:CI18"/>
+    <mergeCell ref="CJ18:CK18"/>
+    <mergeCell ref="CL18:CM18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="H9 V9 C56:G56 AC11:AY11 AC25:AG25 F58:I58 AZ11 AH25:AJ25 BE25:BF25 BL25 BQ25 CD25:DA25 CN34:CN40 CP34:CP40 CQ34:CQ39 CO34:CO39 CO40 CQ40" formula="1"/>
+    <ignoredError sqref="H9 V9 C56:G56 AC11:AY11 AC25:AG25 F58:I58 AZ11 AH25:AJ25 BE25:BF25 BL25 BQ25 CD25:DA25 CN34:CN40 CP34:CP40 CQ34:CQ39 CO34:CO39 CO40 CQ40 AJ58 AH58 AF58" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>